<commit_message>
added excel with distances and in code
</commit_message>
<xml_diff>
--- a/testees.xlsx
+++ b/testees.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikvanbaasbank\PycharmProjects\Operations_JoshLiesErik\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liesbethwijn/PycharmProjects/Operations_JoshLiesErik/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED52C076-6C3F-472D-8744-741B0B280FD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="4560" windowWidth="21600" windowHeight="11385" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3820" yWindow="3760" windowWidth="21600" windowHeight="11380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RandomPopulation" sheetId="1" r:id="rId1"/>
-    <sheet name="StedenInformatie" sheetId="2" r:id="rId2"/>
-    <sheet name="Costst" sheetId="3" r:id="rId3"/>
+    <sheet name="distancetable" sheetId="4" r:id="rId2"/>
+    <sheet name="StedenInformatie" sheetId="2" r:id="rId3"/>
+    <sheet name="Costst" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -28,9 +31,6 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -178,13 +178,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -465,14 +465,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -698,7 +698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -706,7 +706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -714,7 +714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -722,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2</v>
       </c>
@@ -730,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -738,7 +738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -746,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -754,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -762,7 +762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2</v>
       </c>
@@ -770,7 +770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3</v>
       </c>
@@ -778,7 +778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2</v>
       </c>
@@ -786,7 +786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2</v>
       </c>
@@ -794,7 +794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -802,7 +802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -810,7 +810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2</v>
       </c>
@@ -818,7 +818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2</v>
       </c>
@@ -826,7 +826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3</v>
       </c>
@@ -834,7 +834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3</v>
       </c>
@@ -842,7 +842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2</v>
       </c>
@@ -850,7 +850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2</v>
       </c>
@@ -858,7 +858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3</v>
       </c>
@@ -866,7 +866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2</v>
       </c>
@@ -874,7 +874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1</v>
       </c>
@@ -882,7 +882,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2</v>
       </c>
@@ -890,7 +890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1</v>
       </c>
@@ -898,7 +898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2</v>
       </c>
@@ -906,7 +906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2</v>
       </c>
@@ -914,7 +914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>3</v>
       </c>
@@ -922,7 +922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>3</v>
       </c>
@@ -930,7 +930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2</v>
       </c>
@@ -938,7 +938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2</v>
       </c>
@@ -946,7 +946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1</v>
       </c>
@@ -960,33 +960,469 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0FFC0C-9CB5-4752-A823-CFBA782F28A3}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="7" max="7" width="10.375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>57.6</v>
+      </c>
+      <c r="C1">
+        <v>25.760000000000005</v>
+      </c>
+      <c r="D1">
+        <v>47.6</v>
+      </c>
+      <c r="E1">
+        <v>70</v>
+      </c>
+      <c r="F1">
+        <v>46</v>
+      </c>
+      <c r="G1">
+        <v>64</v>
+      </c>
+      <c r="H1">
+        <v>39.760000000000005</v>
+      </c>
+      <c r="I1">
+        <v>63.6</v>
+      </c>
+      <c r="J1">
+        <v>84</v>
+      </c>
+      <c r="K1">
+        <v>26.04</v>
+      </c>
+      <c r="L1">
+        <v>27.400000000000002</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>57.6</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>81.600000000000009</v>
+      </c>
+      <c r="D2">
+        <v>91.2</v>
+      </c>
+      <c r="E2">
+        <v>12.440000000000001</v>
+      </c>
+      <c r="F2">
+        <v>82.4</v>
+      </c>
+      <c r="G2">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="H2">
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>122.80000000000001</v>
+      </c>
+      <c r="J2">
+        <v>132.4</v>
+      </c>
+      <c r="K2">
+        <v>66</v>
+      </c>
+      <c r="L2">
+        <v>30.200000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>25.760000000000005</v>
+      </c>
+      <c r="B3">
+        <v>81.600000000000009</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>42.800000000000004</v>
+      </c>
+      <c r="E3">
+        <v>94.4</v>
+      </c>
+      <c r="F3">
+        <v>40.800000000000004</v>
+      </c>
+      <c r="G3">
+        <v>83.2</v>
+      </c>
+      <c r="H3">
+        <v>45.2</v>
+      </c>
+      <c r="I3">
+        <v>50.400000000000006</v>
+      </c>
+      <c r="J3">
+        <v>60</v>
+      </c>
+      <c r="K3">
+        <v>22.400000000000002</v>
+      </c>
+      <c r="L3">
+        <v>51.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>47.6</v>
+      </c>
+      <c r="B4">
+        <v>91.2</v>
+      </c>
+      <c r="C4">
+        <v>42.800000000000004</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>94.4</v>
+      </c>
+      <c r="F4">
+        <v>23.680000000000003</v>
+      </c>
+      <c r="G4">
+        <v>77.2</v>
+      </c>
+      <c r="H4">
+        <v>45.2</v>
+      </c>
+      <c r="I4">
+        <v>92.4</v>
+      </c>
+      <c r="J4">
+        <v>45.6</v>
+      </c>
+      <c r="K4">
+        <v>27.680000000000003</v>
+      </c>
+      <c r="L4">
+        <v>61.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>70</v>
+      </c>
+      <c r="B5">
+        <v>12.440000000000001</v>
+      </c>
+      <c r="C5">
+        <v>94.4</v>
+      </c>
+      <c r="D5">
+        <v>94.4</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>80.800000000000011</v>
+      </c>
+      <c r="G5">
+        <v>25.84</v>
+      </c>
+      <c r="H5">
+        <v>51.2</v>
+      </c>
+      <c r="I5">
+        <v>134.4</v>
+      </c>
+      <c r="J5">
+        <v>142</v>
+      </c>
+      <c r="K5">
+        <v>75.2</v>
+      </c>
+      <c r="L5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>82.4</v>
+      </c>
+      <c r="C6">
+        <v>40.800000000000004</v>
+      </c>
+      <c r="D6">
+        <v>23.680000000000003</v>
+      </c>
+      <c r="E6">
+        <v>80.800000000000011</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>56.400000000000006</v>
+      </c>
+      <c r="H6">
+        <v>32.04</v>
+      </c>
+      <c r="I6">
+        <v>91.2</v>
+      </c>
+      <c r="J6">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="K6">
+        <v>24.040000000000003</v>
+      </c>
+      <c r="L6">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>64</v>
+      </c>
+      <c r="B7">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="C7">
+        <v>83.2</v>
+      </c>
+      <c r="D7">
+        <v>77.2</v>
+      </c>
+      <c r="E7">
+        <v>25.84</v>
+      </c>
+      <c r="F7">
+        <v>56.400000000000006</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>39.360000000000007</v>
+      </c>
+      <c r="I7">
+        <v>129.6</v>
+      </c>
+      <c r="J7">
+        <v>130.4</v>
+      </c>
+      <c r="K7">
+        <v>63.2</v>
+      </c>
+      <c r="L7">
+        <v>36.800000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>39.760000000000005</v>
+      </c>
+      <c r="B8">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>45.2</v>
+      </c>
+      <c r="D8">
+        <v>45.2</v>
+      </c>
+      <c r="E8">
+        <v>51.2</v>
+      </c>
+      <c r="F8">
+        <v>32.04</v>
+      </c>
+      <c r="G8">
+        <v>39.360000000000007</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>95.2</v>
+      </c>
+      <c r="J8">
+        <v>92.800000000000011</v>
+      </c>
+      <c r="K8">
+        <v>25.64</v>
+      </c>
+      <c r="L8">
+        <v>20.560000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>63.6</v>
+      </c>
+      <c r="B9">
+        <v>122.80000000000001</v>
+      </c>
+      <c r="C9">
+        <v>50.400000000000006</v>
+      </c>
+      <c r="D9">
+        <v>92.4</v>
+      </c>
+      <c r="E9">
+        <v>134.4</v>
+      </c>
+      <c r="F9">
+        <v>91.2</v>
+      </c>
+      <c r="G9">
+        <v>129.6</v>
+      </c>
+      <c r="H9">
+        <v>95.2</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>74.8</v>
+      </c>
+      <c r="K9">
+        <v>72</v>
+      </c>
+      <c r="L9">
+        <v>92.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>84</v>
+      </c>
+      <c r="B10">
+        <v>132.4</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>45.6</v>
+      </c>
+      <c r="E10">
+        <v>142</v>
+      </c>
+      <c r="F10">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="G10">
+        <v>130.4</v>
+      </c>
+      <c r="H10">
+        <v>92.800000000000011</v>
+      </c>
+      <c r="I10">
+        <v>74.8</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>68</v>
+      </c>
+      <c r="L10">
+        <v>100.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>26.04</v>
+      </c>
+      <c r="B11">
+        <v>66</v>
+      </c>
+      <c r="C11">
+        <v>22.400000000000002</v>
+      </c>
+      <c r="D11">
+        <v>27.680000000000003</v>
+      </c>
+      <c r="E11">
+        <v>75.2</v>
+      </c>
+      <c r="F11">
+        <v>24.040000000000003</v>
+      </c>
+      <c r="G11">
+        <v>63.2</v>
+      </c>
+      <c r="H11">
+        <v>25.240000000000002</v>
+      </c>
+      <c r="I11">
+        <v>72</v>
+      </c>
+      <c r="J11">
+        <v>68</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>35.92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>27.400000000000002</v>
+      </c>
+      <c r="B12">
+        <v>30.200000000000003</v>
+      </c>
+      <c r="C12">
+        <v>51.6</v>
+      </c>
+      <c r="D12">
+        <v>61.6</v>
+      </c>
+      <c r="E12">
+        <v>42</v>
+      </c>
+      <c r="F12">
+        <v>53.2</v>
+      </c>
+      <c r="G12">
+        <v>36.800000000000004</v>
+      </c>
+      <c r="H12">
+        <v>20.560000000000002</v>
+      </c>
+      <c r="I12">
+        <v>92.4</v>
+      </c>
+      <c r="J12">
+        <v>100.4</v>
+      </c>
+      <c r="K12">
+        <v>35.92</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -995,236 +1431,271 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E9E72C-1F86-4D90-9C9C-A8E9FB8EACF2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="20.875" customWidth="1"/>
-    <col min="4" max="4" width="17.25" customWidth="1"/>
-    <col min="5" max="5" width="15.75" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>0.2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>1000</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>100</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>1E-4</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <f>0.5*C10</f>
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Edited the excel again
</commit_message>
<xml_diff>
--- a/testees.xlsx
+++ b/testees.xlsx
@@ -1,27 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liesbethwijn/PycharmProjects/Operations_JoshLiesErik/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikvanbaasbank\PycharmProjects\Operations_JoshLiesErik\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C6E27E-4DF0-4078-B674-3A8003FD858D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3820" yWindow="3760" windowWidth="21600" windowHeight="11380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RandomPopulation" sheetId="1" r:id="rId1"/>
-    <sheet name="distancetable" sheetId="4" r:id="rId2"/>
-    <sheet name="StedenInformatie" sheetId="2" r:id="rId3"/>
-    <sheet name="Costst" sheetId="3" r:id="rId4"/>
+    <sheet name="StedenInformatie" sheetId="5" r:id="rId2"/>
+    <sheet name="Costs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>timepref</t>
   </si>
@@ -104,9 +101,6 @@
     <t>Inwoners</t>
   </si>
   <si>
-    <t>Zieken</t>
-  </si>
-  <si>
     <t>C4</t>
   </si>
   <si>
@@ -129,15 +123,67 @@
   </si>
   <si>
     <t>eu</t>
+  </si>
+  <si>
+    <t>Groningen</t>
+  </si>
+  <si>
+    <t>Leeuwarden</t>
+  </si>
+  <si>
+    <t>Assen</t>
+  </si>
+  <si>
+    <t>Zwolle</t>
+  </si>
+  <si>
+    <t>Arnhem</t>
+  </si>
+  <si>
+    <t>Haarlem</t>
+  </si>
+  <si>
+    <t>Middelburg</t>
+  </si>
+  <si>
+    <t>Maastricht</t>
+  </si>
+  <si>
+    <t>Lelystad</t>
+  </si>
+  <si>
+    <t>Den Haag</t>
+  </si>
+  <si>
+    <t>Den Bosch</t>
+  </si>
+  <si>
+    <t>Testees</t>
+  </si>
+  <si>
+    <t>Treshold for opening up</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -150,6 +196,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -169,10 +220,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -180,15 +244,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="14">
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{6396D736-435B-4CE9-9573-A35C48AE74DC}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{654D7B34-106A-43AF-8243-234D3C28E9E0}"/>
+    <cellStyle name="Procent 2" xfId="4" xr:uid="{F743ED5D-DD3C-4BEB-9641-73FDA783069D}"/>
+    <cellStyle name="Standaard 2" xfId="3" xr:uid="{30AFE39D-D777-4D2A-A9B8-5DE8E1AB8CFA}"/>
+    <cellStyle name="Standaard 2 2" xfId="12" xr:uid="{5BC5D56A-67FD-4300-9768-D377C7A8E3C4}"/>
+    <cellStyle name="Standaard 3" xfId="5" xr:uid="{73566C79-E4E5-43E9-9CF4-4B01EAED8ED4}"/>
+    <cellStyle name="Standaard 4" xfId="13" xr:uid="{6B91E64F-3A6C-4743-BAF4-7663A423F074}"/>
+    <cellStyle name="Standaard_Blad1" xfId="11" xr:uid="{BC12015D-B0D7-48DA-9470-7DEFFC355377}"/>
+    <cellStyle name="style1499936711542" xfId="6" xr:uid="{1F7AAF00-C608-4C1F-8F15-EDD52D46120C}"/>
+    <cellStyle name="style1499936711557" xfId="7" xr:uid="{A2A69F56-9461-425C-BD9D-7376BBB6AD8A}"/>
+    <cellStyle name="style1499936711635" xfId="8" xr:uid="{FD2EC5E1-5A9D-4699-9300-F8EB32CA61D6}"/>
+    <cellStyle name="style1499936711651" xfId="9" xr:uid="{D2B58641-22C2-4BE8-A097-246A25F5D73A}"/>
+    <cellStyle name="style1499936712276" xfId="10" xr:uid="{780714A6-C888-4B36-81D1-83E24DDBB746}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -465,14 +543,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -698,7 +776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -706,7 +784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -714,7 +792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -722,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2</v>
       </c>
@@ -730,7 +808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -738,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -746,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -754,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -762,7 +840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -770,7 +848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -778,7 +856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -786,7 +864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
@@ -794,7 +872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -802,7 +880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -810,7 +888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
@@ -818,7 +896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -826,7 +904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -834,7 +912,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -842,7 +920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2</v>
       </c>
@@ -850,7 +928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
@@ -858,7 +936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
@@ -866,7 +944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2</v>
       </c>
@@ -874,7 +952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1</v>
       </c>
@@ -882,7 +960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2</v>
       </c>
@@ -890,7 +968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1</v>
       </c>
@@ -898,7 +976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2</v>
       </c>
@@ -906,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2</v>
       </c>
@@ -914,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
@@ -922,7 +1000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3</v>
       </c>
@@ -930,7 +1008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2</v>
       </c>
@@ -938,7 +1016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2</v>
       </c>
@@ -946,7 +1024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1</v>
       </c>
@@ -960,469 +1038,223 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181B223E-34D0-4054-AA2D-B7B89630CCD9}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>57.6</v>
-      </c>
-      <c r="C1">
-        <v>25.760000000000005</v>
-      </c>
-      <c r="D1">
-        <v>47.6</v>
-      </c>
-      <c r="E1">
-        <v>70</v>
-      </c>
-      <c r="F1">
-        <v>46</v>
-      </c>
-      <c r="G1">
-        <v>64</v>
-      </c>
-      <c r="H1">
-        <v>39.760000000000005</v>
-      </c>
-      <c r="I1">
-        <v>63.6</v>
-      </c>
-      <c r="J1">
-        <v>84</v>
-      </c>
-      <c r="K1">
-        <v>26.04</v>
-      </c>
-      <c r="L1">
-        <v>27.400000000000002</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>57.6</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>202000</v>
       </c>
       <c r="C2">
-        <v>81.600000000000009</v>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B2)</f>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>91.2</v>
-      </c>
-      <c r="E2">
-        <v>12.440000000000001</v>
-      </c>
-      <c r="F2">
-        <v>82.4</v>
-      </c>
-      <c r="G2">
-        <v>32.880000000000003</v>
-      </c>
-      <c r="H2">
-        <v>50</v>
-      </c>
-      <c r="I2">
-        <v>122.80000000000001</v>
-      </c>
-      <c r="J2">
-        <v>132.4</v>
-      </c>
-      <c r="K2">
-        <v>66</v>
-      </c>
-      <c r="L2">
-        <v>30.200000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>25.760000000000005</v>
+        <f>_xlfn.FLOOR.MATH(0.5*C2)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
       </c>
       <c r="B3">
-        <v>81.600000000000009</v>
+        <v>96000</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B3)</f>
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>42.800000000000004</v>
-      </c>
-      <c r="E3">
-        <v>94.4</v>
-      </c>
-      <c r="F3">
-        <v>40.800000000000004</v>
-      </c>
-      <c r="G3">
-        <v>83.2</v>
-      </c>
-      <c r="H3">
-        <v>45.2</v>
-      </c>
-      <c r="I3">
-        <v>50.400000000000006</v>
-      </c>
-      <c r="J3">
-        <v>60</v>
-      </c>
-      <c r="K3">
-        <v>22.400000000000002</v>
-      </c>
-      <c r="L3">
-        <v>51.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>47.6</v>
+        <f t="shared" ref="D3:D13" si="0">_xlfn.FLOOR.MATH(0.5*C3)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
       </c>
       <c r="B4">
-        <v>91.2</v>
+        <v>67000</v>
       </c>
       <c r="C4">
-        <v>42.800000000000004</v>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B4)</f>
+        <v>6</v>
       </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>94.4</v>
-      </c>
-      <c r="F4">
-        <v>23.680000000000003</v>
-      </c>
-      <c r="G4">
-        <v>77.2</v>
-      </c>
-      <c r="H4">
-        <v>45.2</v>
-      </c>
-      <c r="I4">
-        <v>92.4</v>
-      </c>
-      <c r="J4">
-        <v>45.6</v>
-      </c>
-      <c r="K4">
-        <v>27.680000000000003</v>
-      </c>
-      <c r="L4">
-        <v>61.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>70</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
       </c>
       <c r="B5">
-        <v>12.440000000000001</v>
+        <v>76000</v>
       </c>
       <c r="C5">
-        <v>94.4</v>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B5)</f>
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>94.4</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>80.800000000000011</v>
-      </c>
-      <c r="G5">
-        <v>25.84</v>
-      </c>
-      <c r="H5">
-        <v>51.2</v>
-      </c>
-      <c r="I5">
-        <v>134.4</v>
-      </c>
-      <c r="J5">
-        <v>142</v>
-      </c>
-      <c r="K5">
-        <v>75.2</v>
-      </c>
-      <c r="L5">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>46</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
       </c>
       <c r="B6">
-        <v>82.4</v>
+        <v>123000</v>
       </c>
       <c r="C6">
-        <v>40.800000000000004</v>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B6)</f>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>23.680000000000003</v>
-      </c>
-      <c r="E6">
-        <v>80.800000000000011</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>56.400000000000006</v>
-      </c>
-      <c r="H6">
-        <v>32.04</v>
-      </c>
-      <c r="I6">
-        <v>91.2</v>
-      </c>
-      <c r="J6">
-        <v>66.400000000000006</v>
-      </c>
-      <c r="K6">
-        <v>24.040000000000003</v>
-      </c>
-      <c r="L6">
-        <v>53.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>64</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
       </c>
       <c r="B7">
-        <v>32.880000000000003</v>
+        <v>154000</v>
       </c>
       <c r="C7">
-        <v>83.2</v>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B7)</f>
+        <v>15</v>
       </c>
       <c r="D7">
-        <v>77.2</v>
-      </c>
-      <c r="E7">
-        <v>25.84</v>
-      </c>
-      <c r="F7">
-        <v>56.400000000000006</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>39.360000000000007</v>
-      </c>
-      <c r="I7">
-        <v>129.6</v>
-      </c>
-      <c r="J7">
-        <v>130.4</v>
-      </c>
-      <c r="K7">
-        <v>63.2</v>
-      </c>
-      <c r="L7">
-        <v>36.800000000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>39.760000000000005</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>353000</v>
       </c>
       <c r="C8">
-        <v>45.2</v>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B8)</f>
+        <v>35</v>
       </c>
       <c r="D8">
-        <v>45.2</v>
-      </c>
-      <c r="E8">
-        <v>51.2</v>
-      </c>
-      <c r="F8">
-        <v>32.04</v>
-      </c>
-      <c r="G8">
-        <v>39.360000000000007</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>95.2</v>
-      </c>
-      <c r="J8">
-        <v>92.800000000000011</v>
-      </c>
-      <c r="K8">
-        <v>25.64</v>
-      </c>
-      <c r="L8">
-        <v>20.560000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>63.6</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
       </c>
       <c r="B9">
-        <v>122.80000000000001</v>
+        <v>538000</v>
       </c>
       <c r="C9">
-        <v>50.400000000000006</v>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B9)</f>
+        <v>53</v>
       </c>
       <c r="D9">
-        <v>92.4</v>
-      </c>
-      <c r="E9">
-        <v>134.4</v>
-      </c>
-      <c r="F9">
-        <v>91.2</v>
-      </c>
-      <c r="G9">
-        <v>129.6</v>
-      </c>
-      <c r="H9">
-        <v>95.2</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>74.8</v>
-      </c>
-      <c r="K9">
-        <v>72</v>
-      </c>
-      <c r="L9">
-        <v>92.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>84</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
       </c>
       <c r="B10">
-        <v>132.4</v>
+        <v>150000</v>
       </c>
       <c r="C10">
-        <v>60</v>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B10)</f>
+        <v>15</v>
       </c>
       <c r="D10">
-        <v>45.6</v>
-      </c>
-      <c r="E10">
-        <v>142</v>
-      </c>
-      <c r="F10">
-        <v>66.400000000000006</v>
-      </c>
-      <c r="G10">
-        <v>130.4</v>
-      </c>
-      <c r="H10">
-        <v>92.800000000000011</v>
-      </c>
-      <c r="I10">
-        <v>74.8</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>68</v>
-      </c>
-      <c r="L10">
-        <v>100.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>26.04</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
       </c>
       <c r="B11">
-        <v>66</v>
+        <v>143000</v>
       </c>
       <c r="C11">
-        <v>22.400000000000002</v>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B11)</f>
+        <v>14</v>
       </c>
       <c r="D11">
-        <v>27.680000000000003</v>
-      </c>
-      <c r="E11">
-        <v>75.2</v>
-      </c>
-      <c r="F11">
-        <v>24.040000000000003</v>
-      </c>
-      <c r="G11">
-        <v>63.2</v>
-      </c>
-      <c r="H11">
-        <v>25.240000000000002</v>
-      </c>
-      <c r="I11">
-        <v>72</v>
-      </c>
-      <c r="J11">
-        <v>68</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>35.92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>27.400000000000002</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
       </c>
       <c r="B12">
-        <v>30.200000000000003</v>
+        <v>47700</v>
       </c>
       <c r="C12">
-        <v>51.6</v>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B12)</f>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>61.6</v>
-      </c>
-      <c r="E12">
-        <v>42</v>
-      </c>
-      <c r="F12">
-        <v>53.2</v>
-      </c>
-      <c r="G12">
-        <v>36.800000000000004</v>
-      </c>
-      <c r="H12">
-        <v>20.560000000000002</v>
-      </c>
-      <c r="I12">
-        <v>92.4</v>
-      </c>
-      <c r="J12">
-        <v>100.4</v>
-      </c>
-      <c r="K12">
-        <v>35.92</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <v>121000</v>
+      </c>
+      <c r="C13">
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B13)</f>
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1431,82 +1263,47 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E9E72C-1F86-4D90-9C9C-A8E9FB8EACF2}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D14" sqref="D14:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.875" customWidth="1"/>
+    <col min="4" max="4" width="17.25" customWidth="1"/>
+    <col min="5" max="5" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1514,188 +1311,187 @@
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>0.2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>1000</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <v>100</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="C12" s="4">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="3">
-        <f>0.5*C10</f>
-        <v>5.0000000000000002E-5</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
distance table in excel
</commit_message>
<xml_diff>
--- a/testees.xlsx
+++ b/testees.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26124"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikvanbaasbank\PycharmProjects\Operations_JoshLiesErik\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liesbethwijn/PycharmProjects/Operations_JoshLiesErik/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C6E27E-4DF0-4078-B674-3A8003FD858D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RandomPopulation" sheetId="1" r:id="rId1"/>
     <sheet name="StedenInformatie" sheetId="5" r:id="rId2"/>
     <sheet name="Costs" sheetId="3" r:id="rId3"/>
+    <sheet name="distancetable" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -170,7 +173,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -253,20 +256,20 @@
     </xf>
   </cellXfs>
   <cellStyles count="14">
-    <cellStyle name="Comma 2" xfId="2" xr:uid="{6396D736-435B-4CE9-9573-A35C48AE74DC}"/>
+    <cellStyle name="Comma 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{654D7B34-106A-43AF-8243-234D3C28E9E0}"/>
-    <cellStyle name="Procent 2" xfId="4" xr:uid="{F743ED5D-DD3C-4BEB-9641-73FDA783069D}"/>
-    <cellStyle name="Standaard 2" xfId="3" xr:uid="{30AFE39D-D777-4D2A-A9B8-5DE8E1AB8CFA}"/>
-    <cellStyle name="Standaard 2 2" xfId="12" xr:uid="{5BC5D56A-67FD-4300-9768-D377C7A8E3C4}"/>
-    <cellStyle name="Standaard 3" xfId="5" xr:uid="{73566C79-E4E5-43E9-9CF4-4B01EAED8ED4}"/>
-    <cellStyle name="Standaard 4" xfId="13" xr:uid="{6B91E64F-3A6C-4743-BAF4-7663A423F074}"/>
-    <cellStyle name="Standaard_Blad1" xfId="11" xr:uid="{BC12015D-B0D7-48DA-9470-7DEFFC355377}"/>
-    <cellStyle name="style1499936711542" xfId="6" xr:uid="{1F7AAF00-C608-4C1F-8F15-EDD52D46120C}"/>
-    <cellStyle name="style1499936711557" xfId="7" xr:uid="{A2A69F56-9461-425C-BD9D-7376BBB6AD8A}"/>
-    <cellStyle name="style1499936711635" xfId="8" xr:uid="{FD2EC5E1-5A9D-4699-9300-F8EB32CA61D6}"/>
-    <cellStyle name="style1499936711651" xfId="9" xr:uid="{D2B58641-22C2-4BE8-A097-246A25F5D73A}"/>
-    <cellStyle name="style1499936712276" xfId="10" xr:uid="{780714A6-C888-4B36-81D1-83E24DDBB746}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Procent 2" xfId="4"/>
+    <cellStyle name="Standaard 2" xfId="3"/>
+    <cellStyle name="Standaard 2 2" xfId="12"/>
+    <cellStyle name="Standaard 3" xfId="5"/>
+    <cellStyle name="Standaard 4" xfId="13"/>
+    <cellStyle name="Standaard_Blad1" xfId="11"/>
+    <cellStyle name="style1499936711542" xfId="6"/>
+    <cellStyle name="style1499936711557" xfId="7"/>
+    <cellStyle name="style1499936711635" xfId="8"/>
+    <cellStyle name="style1499936711651" xfId="9"/>
+    <cellStyle name="style1499936712276" xfId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -543,14 +546,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -864,7 +867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2</v>
       </c>
@@ -872,7 +875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -880,7 +883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -888,7 +891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2</v>
       </c>
@@ -896,7 +899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2</v>
       </c>
@@ -904,7 +907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3</v>
       </c>
@@ -912,7 +915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3</v>
       </c>
@@ -920,7 +923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2</v>
       </c>
@@ -928,7 +931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2</v>
       </c>
@@ -936,7 +939,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3</v>
       </c>
@@ -944,7 +947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2</v>
       </c>
@@ -952,7 +955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1</v>
       </c>
@@ -960,7 +963,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2</v>
       </c>
@@ -968,7 +971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1</v>
       </c>
@@ -976,7 +979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2</v>
       </c>
@@ -984,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2</v>
       </c>
@@ -992,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>3</v>
       </c>
@@ -1000,7 +1003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>3</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2</v>
       </c>
@@ -1016,7 +1019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2</v>
       </c>
@@ -1024,7 +1027,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1</v>
       </c>
@@ -1038,14 +1041,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181B223E-34D0-4054-AA2D-B7B89630CCD9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
@@ -1263,23 +1266,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E9E72C-1F86-4D90-9C9C-A8E9FB8EACF2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="20.875" customWidth="1"/>
-    <col min="4" max="4" width="17.25" customWidth="1"/>
-    <col min="5" max="5" width="15.75" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>4</v>
@@ -1295,7 +1298,7 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1303,7 +1306,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1311,7 +1314,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1329,7 +1332,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1337,7 +1340,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1355,7 +1358,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1363,7 +1366,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -1381,7 +1384,7 @@
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1389,7 +1392,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
@@ -1404,14 +1407,14 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -1426,14 +1429,14 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -1448,7 +1451,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1457,42 +1460,513 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>57.6</v>
+      </c>
+      <c r="C1">
+        <v>25.760000000000005</v>
+      </c>
+      <c r="D1">
+        <v>47.6</v>
+      </c>
+      <c r="E1">
+        <v>70</v>
+      </c>
+      <c r="F1">
+        <v>46</v>
+      </c>
+      <c r="G1">
+        <v>64</v>
+      </c>
+      <c r="H1">
+        <v>39.760000000000005</v>
+      </c>
+      <c r="I1">
+        <v>63.6</v>
+      </c>
+      <c r="J1">
+        <v>84</v>
+      </c>
+      <c r="K1">
+        <v>26.04</v>
+      </c>
+      <c r="L1">
+        <v>27.400000000000002</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>57.6</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>81.600000000000009</v>
+      </c>
+      <c r="D2">
+        <v>91.2</v>
+      </c>
+      <c r="E2">
+        <v>12.440000000000001</v>
+      </c>
+      <c r="F2">
+        <v>82.4</v>
+      </c>
+      <c r="G2">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="H2">
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>122.80000000000001</v>
+      </c>
+      <c r="J2">
+        <v>132.4</v>
+      </c>
+      <c r="K2">
+        <v>66</v>
+      </c>
+      <c r="L2">
+        <v>30.200000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>25.760000000000005</v>
+      </c>
+      <c r="B3">
+        <v>81.600000000000009</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>42.800000000000004</v>
+      </c>
+      <c r="E3">
+        <v>94.4</v>
+      </c>
+      <c r="F3">
+        <v>40.800000000000004</v>
+      </c>
+      <c r="G3">
+        <v>83.2</v>
+      </c>
+      <c r="H3">
+        <v>45.2</v>
+      </c>
+      <c r="I3">
+        <v>50.400000000000006</v>
+      </c>
+      <c r="J3">
+        <v>60</v>
+      </c>
+      <c r="K3">
+        <v>22.400000000000002</v>
+      </c>
+      <c r="L3">
+        <v>51.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>47.6</v>
+      </c>
+      <c r="B4">
+        <v>91.2</v>
+      </c>
+      <c r="C4">
+        <v>42.800000000000004</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>94.4</v>
+      </c>
+      <c r="F4">
+        <v>23.680000000000003</v>
+      </c>
+      <c r="G4">
+        <v>77.2</v>
+      </c>
+      <c r="H4">
+        <v>45.2</v>
+      </c>
+      <c r="I4">
+        <v>92.4</v>
+      </c>
+      <c r="J4">
+        <v>45.6</v>
+      </c>
+      <c r="K4">
+        <v>27.680000000000003</v>
+      </c>
+      <c r="L4">
+        <v>61.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>70</v>
+      </c>
+      <c r="B5">
+        <v>12.440000000000001</v>
+      </c>
+      <c r="C5">
+        <v>94.4</v>
+      </c>
+      <c r="D5">
+        <v>94.4</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>80.800000000000011</v>
+      </c>
+      <c r="G5">
+        <v>25.84</v>
+      </c>
+      <c r="H5">
+        <v>51.2</v>
+      </c>
+      <c r="I5">
+        <v>134.4</v>
+      </c>
+      <c r="J5">
+        <v>142</v>
+      </c>
+      <c r="K5">
+        <v>75.2</v>
+      </c>
+      <c r="L5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>82.4</v>
+      </c>
+      <c r="C6">
+        <v>40.800000000000004</v>
+      </c>
+      <c r="D6">
+        <v>23.680000000000003</v>
+      </c>
+      <c r="E6">
+        <v>80.800000000000011</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>56.400000000000006</v>
+      </c>
+      <c r="H6">
+        <v>32.04</v>
+      </c>
+      <c r="I6">
+        <v>91.2</v>
+      </c>
+      <c r="J6">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="K6">
+        <v>24.040000000000003</v>
+      </c>
+      <c r="L6">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>64</v>
+      </c>
+      <c r="B7">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="C7">
+        <v>83.2</v>
+      </c>
+      <c r="D7">
+        <v>77.2</v>
+      </c>
+      <c r="E7">
+        <v>25.84</v>
+      </c>
+      <c r="F7">
+        <v>56.400000000000006</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>39.360000000000007</v>
+      </c>
+      <c r="I7">
+        <v>129.6</v>
+      </c>
+      <c r="J7">
+        <v>130.4</v>
+      </c>
+      <c r="K7">
+        <v>63.2</v>
+      </c>
+      <c r="L7">
+        <v>36.800000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>39.760000000000005</v>
+      </c>
+      <c r="B8">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>45.2</v>
+      </c>
+      <c r="D8">
+        <v>45.2</v>
+      </c>
+      <c r="E8">
+        <v>51.2</v>
+      </c>
+      <c r="F8">
+        <v>32.04</v>
+      </c>
+      <c r="G8">
+        <v>39.360000000000007</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>95.2</v>
+      </c>
+      <c r="J8">
+        <v>92.800000000000011</v>
+      </c>
+      <c r="K8">
+        <v>25.64</v>
+      </c>
+      <c r="L8">
+        <v>20.560000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>63.6</v>
+      </c>
+      <c r="B9">
+        <v>122.80000000000001</v>
+      </c>
+      <c r="C9">
+        <v>50.400000000000006</v>
+      </c>
+      <c r="D9">
+        <v>92.4</v>
+      </c>
+      <c r="E9">
+        <v>134.4</v>
+      </c>
+      <c r="F9">
+        <v>91.2</v>
+      </c>
+      <c r="G9">
+        <v>129.6</v>
+      </c>
+      <c r="H9">
+        <v>95.2</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>74.8</v>
+      </c>
+      <c r="K9">
+        <v>72</v>
+      </c>
+      <c r="L9">
+        <v>92.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>84</v>
+      </c>
+      <c r="B10">
+        <v>132.4</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>45.6</v>
+      </c>
+      <c r="E10">
+        <v>142</v>
+      </c>
+      <c r="F10">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="G10">
+        <v>130.4</v>
+      </c>
+      <c r="H10">
+        <v>92.800000000000011</v>
+      </c>
+      <c r="I10">
+        <v>74.8</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>68</v>
+      </c>
+      <c r="L10">
+        <v>100.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>26.04</v>
+      </c>
+      <c r="B11">
+        <v>66</v>
+      </c>
+      <c r="C11">
+        <v>22.400000000000002</v>
+      </c>
+      <c r="D11">
+        <v>27.680000000000003</v>
+      </c>
+      <c r="E11">
+        <v>75.2</v>
+      </c>
+      <c r="F11">
+        <v>24.040000000000003</v>
+      </c>
+      <c r="G11">
+        <v>63.2</v>
+      </c>
+      <c r="H11">
+        <v>25.240000000000002</v>
+      </c>
+      <c r="I11">
+        <v>72</v>
+      </c>
+      <c r="J11">
+        <v>68</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>35.92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>27.400000000000002</v>
+      </c>
+      <c r="B12">
+        <v>30.200000000000003</v>
+      </c>
+      <c r="C12">
+        <v>51.6</v>
+      </c>
+      <c r="D12">
+        <v>61.6</v>
+      </c>
+      <c r="E12">
+        <v>42</v>
+      </c>
+      <c r="F12">
+        <v>53.2</v>
+      </c>
+      <c r="G12">
+        <v>36.800000000000004</v>
+      </c>
+      <c r="H12">
+        <v>20.560000000000002</v>
+      </c>
+      <c r="I12">
+        <v>92.4</v>
+      </c>
+      <c r="J12">
+        <v>100.4</v>
+      </c>
+      <c r="K12">
+        <v>35.92</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Edited the excel again again
</commit_message>
<xml_diff>
--- a/testees.xlsx
+++ b/testees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikvanbaasbank\PycharmProjects\Operations_JoshLiesErik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C6E27E-4DF0-4078-B674-3A8003FD858D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46E9FB9-5EBB-4E65-AA45-32E322D6B89F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RandomPopulation" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>timepref</t>
   </si>
@@ -41,9 +41,6 @@
     <t>livloc</t>
   </si>
   <si>
-    <t>Stad</t>
-  </si>
-  <si>
     <t>Utrecht</t>
   </si>
   <si>
@@ -165,6 +162,12 @@
   </si>
   <si>
     <t>p</t>
+  </si>
+  <si>
+    <t>Stad_naam</t>
+  </si>
+  <si>
+    <t>LL</t>
   </si>
 </sst>
 </file>
@@ -236,7 +239,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -250,6 +253,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -546,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1039,222 +1045,256 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181B223E-34D0-4054-AA2D-B7B89630CCD9}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="5" max="5" width="23.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>202000</v>
+      </c>
+      <c r="D2">
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C2)</f>
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="B2">
-        <v>202000</v>
-      </c>
-      <c r="C2">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B2)</f>
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <f>_xlfn.FLOOR.MATH(0.5*C2)</f>
+      <c r="C3">
+        <v>96000</v>
+      </c>
+      <c r="D3">
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C3)</f>
+        <v>9</v>
+      </c>
+      <c r="E3">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="B3">
-        <v>96000</v>
-      </c>
-      <c r="C3">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B3)</f>
+      <c r="C4">
+        <v>67000</v>
+      </c>
+      <c r="D4">
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C4)</f>
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5">
+        <v>76000</v>
+      </c>
+      <c r="D5">
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C5)</f>
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>123000</v>
+      </c>
+      <c r="D6">
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C6)</f>
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7">
+        <v>154000</v>
+      </c>
+      <c r="D7">
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C7)</f>
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>353000</v>
+      </c>
+      <c r="D8">
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C8)</f>
+        <v>35</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9">
+        <v>538000</v>
+      </c>
+      <c r="D9">
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C9)</f>
+        <v>53</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D13" si="0">_xlfn.FLOOR.MATH(0.5*C3)</f>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>150000</v>
+      </c>
+      <c r="D10">
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C10)</f>
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11">
+        <v>143000</v>
+      </c>
+      <c r="D11">
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C11)</f>
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>47700</v>
+      </c>
+      <c r="D12">
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C12)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4">
-        <v>67000</v>
-      </c>
-      <c r="C4">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B4)</f>
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5">
-        <v>76000</v>
-      </c>
-      <c r="C5">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B5)</f>
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6">
-        <v>123000</v>
-      </c>
-      <c r="C6">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B6)</f>
+      <c r="E12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7">
-        <v>154000</v>
-      </c>
-      <c r="C7">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B7)</f>
-        <v>15</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>353000</v>
-      </c>
-      <c r="C8">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B8)</f>
-        <v>35</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9">
-        <v>538000</v>
-      </c>
-      <c r="C9">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B9)</f>
-        <v>53</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10">
-        <v>150000</v>
-      </c>
-      <c r="C10">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B10)</f>
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11">
-        <v>143000</v>
-      </c>
-      <c r="C11">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B11)</f>
-        <v>14</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="B12">
-        <v>47700</v>
-      </c>
-      <c r="C12">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B12)</f>
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13">
+      <c r="C13">
         <v>121000</v>
       </c>
-      <c r="C13">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B13)</f>
+      <c r="D13">
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C13)</f>
         <v>12</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>6</v>
+      <c r="E13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f>SUM(D2:D13)</f>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -1282,16 +1322,16 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="F1" s="2"/>
     </row>
@@ -1313,19 +1353,19 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="C4" s="4">
         <v>0.2</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1339,19 +1379,19 @@
     </row>
     <row r="6" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="C6" s="4">
         <v>1000</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -1365,19 +1405,19 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="C8" s="4">
         <v>100</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -1391,16 +1431,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="4">
         <v>1E-4</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="4"/>
     </row>
@@ -1413,16 +1453,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="4">
         <v>10</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="4"/>
     </row>
@@ -1435,16 +1475,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="E14" s="4"/>
     </row>
@@ -1457,41 +1497,41 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
distance table in excel en 12 steden + 5 dagen in code
</commit_message>
<xml_diff>
--- a/testees.xlsx
+++ b/testees.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26124"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikvanbaasbank\PycharmProjects\Operations_JoshLiesErik\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liesbethwijn/PycharmProjects/Operations_JoshLiesErik/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46E9FB9-5EBB-4E65-AA45-32E322D6B89F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RandomPopulation" sheetId="1" r:id="rId1"/>
     <sheet name="StedenInformatie" sheetId="5" r:id="rId2"/>
-    <sheet name="Costs" sheetId="3" r:id="rId3"/>
+    <sheet name="distancetable" sheetId="6" r:id="rId3"/>
+    <sheet name="Costs" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -173,7 +176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -248,31 +251,31 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="14">
-    <cellStyle name="Comma 2" xfId="2" xr:uid="{6396D736-435B-4CE9-9573-A35C48AE74DC}"/>
+    <cellStyle name="Comma 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{654D7B34-106A-43AF-8243-234D3C28E9E0}"/>
-    <cellStyle name="Procent 2" xfId="4" xr:uid="{F743ED5D-DD3C-4BEB-9641-73FDA783069D}"/>
-    <cellStyle name="Standaard 2" xfId="3" xr:uid="{30AFE39D-D777-4D2A-A9B8-5DE8E1AB8CFA}"/>
-    <cellStyle name="Standaard 2 2" xfId="12" xr:uid="{5BC5D56A-67FD-4300-9768-D377C7A8E3C4}"/>
-    <cellStyle name="Standaard 3" xfId="5" xr:uid="{73566C79-E4E5-43E9-9CF4-4B01EAED8ED4}"/>
-    <cellStyle name="Standaard 4" xfId="13" xr:uid="{6B91E64F-3A6C-4743-BAF4-7663A423F074}"/>
-    <cellStyle name="Standaard_Blad1" xfId="11" xr:uid="{BC12015D-B0D7-48DA-9470-7DEFFC355377}"/>
-    <cellStyle name="style1499936711542" xfId="6" xr:uid="{1F7AAF00-C608-4C1F-8F15-EDD52D46120C}"/>
-    <cellStyle name="style1499936711557" xfId="7" xr:uid="{A2A69F56-9461-425C-BD9D-7376BBB6AD8A}"/>
-    <cellStyle name="style1499936711635" xfId="8" xr:uid="{FD2EC5E1-5A9D-4699-9300-F8EB32CA61D6}"/>
-    <cellStyle name="style1499936711651" xfId="9" xr:uid="{D2B58641-22C2-4BE8-A097-246A25F5D73A}"/>
-    <cellStyle name="style1499936712276" xfId="10" xr:uid="{780714A6-C888-4B36-81D1-83E24DDBB746}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Procent 2" xfId="4"/>
+    <cellStyle name="Standaard 2" xfId="3"/>
+    <cellStyle name="Standaard 2 2" xfId="12"/>
+    <cellStyle name="Standaard 3" xfId="5"/>
+    <cellStyle name="Standaard 4" xfId="13"/>
+    <cellStyle name="Standaard_Blad1" xfId="11"/>
+    <cellStyle name="style1499936711542" xfId="6"/>
+    <cellStyle name="style1499936711557" xfId="7"/>
+    <cellStyle name="style1499936711635" xfId="8"/>
+    <cellStyle name="style1499936711651" xfId="9"/>
+    <cellStyle name="style1499936712276" xfId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -549,14 +552,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -870,7 +873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2</v>
       </c>
@@ -878,7 +881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -886,7 +889,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -894,7 +897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2</v>
       </c>
@@ -902,7 +905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2</v>
       </c>
@@ -910,7 +913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3</v>
       </c>
@@ -918,7 +921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3</v>
       </c>
@@ -926,7 +929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2</v>
       </c>
@@ -934,7 +937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2</v>
       </c>
@@ -942,7 +945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3</v>
       </c>
@@ -950,7 +953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2</v>
       </c>
@@ -958,7 +961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1</v>
       </c>
@@ -966,7 +969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2</v>
       </c>
@@ -974,7 +977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1</v>
       </c>
@@ -982,7 +985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2</v>
       </c>
@@ -990,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>3</v>
       </c>
@@ -1006,7 +1009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>3</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1</v>
       </c>
@@ -1044,21 +1047,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181B223E-34D0-4054-AA2D-B7B89630CCD9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="5" max="5" width="23.875" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1303,47 +1306,518 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E9E72C-1F86-4D90-9C9C-A8E9FB8EACF2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>57.6</v>
+      </c>
+      <c r="C1">
+        <v>25.760000000000005</v>
+      </c>
+      <c r="D1">
+        <v>47.6</v>
+      </c>
+      <c r="E1">
+        <v>70</v>
+      </c>
+      <c r="F1">
+        <v>46</v>
+      </c>
+      <c r="G1">
+        <v>64</v>
+      </c>
+      <c r="H1">
+        <v>39.760000000000005</v>
+      </c>
+      <c r="I1">
+        <v>63.6</v>
+      </c>
+      <c r="J1">
+        <v>84</v>
+      </c>
+      <c r="K1">
+        <v>26.04</v>
+      </c>
+      <c r="L1">
+        <v>27.400000000000002</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>57.6</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>81.600000000000009</v>
+      </c>
+      <c r="D2">
+        <v>91.2</v>
+      </c>
+      <c r="E2">
+        <v>12.440000000000001</v>
+      </c>
+      <c r="F2">
+        <v>82.4</v>
+      </c>
+      <c r="G2">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="H2">
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>122.80000000000001</v>
+      </c>
+      <c r="J2">
+        <v>132.4</v>
+      </c>
+      <c r="K2">
+        <v>66</v>
+      </c>
+      <c r="L2">
+        <v>30.200000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>25.760000000000005</v>
+      </c>
+      <c r="B3">
+        <v>81.600000000000009</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>42.800000000000004</v>
+      </c>
+      <c r="E3">
+        <v>94.4</v>
+      </c>
+      <c r="F3">
+        <v>40.800000000000004</v>
+      </c>
+      <c r="G3">
+        <v>83.2</v>
+      </c>
+      <c r="H3">
+        <v>45.2</v>
+      </c>
+      <c r="I3">
+        <v>50.400000000000006</v>
+      </c>
+      <c r="J3">
+        <v>60</v>
+      </c>
+      <c r="K3">
+        <v>22.400000000000002</v>
+      </c>
+      <c r="L3">
+        <v>51.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>47.6</v>
+      </c>
+      <c r="B4">
+        <v>91.2</v>
+      </c>
+      <c r="C4">
+        <v>42.800000000000004</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>94.4</v>
+      </c>
+      <c r="F4">
+        <v>23.680000000000003</v>
+      </c>
+      <c r="G4">
+        <v>77.2</v>
+      </c>
+      <c r="H4">
+        <v>45.2</v>
+      </c>
+      <c r="I4">
+        <v>92.4</v>
+      </c>
+      <c r="J4">
+        <v>45.6</v>
+      </c>
+      <c r="K4">
+        <v>27.680000000000003</v>
+      </c>
+      <c r="L4">
+        <v>61.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>70</v>
+      </c>
+      <c r="B5">
+        <v>12.440000000000001</v>
+      </c>
+      <c r="C5">
+        <v>94.4</v>
+      </c>
+      <c r="D5">
+        <v>94.4</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>80.800000000000011</v>
+      </c>
+      <c r="G5">
+        <v>25.84</v>
+      </c>
+      <c r="H5">
+        <v>51.2</v>
+      </c>
+      <c r="I5">
+        <v>134.4</v>
+      </c>
+      <c r="J5">
+        <v>142</v>
+      </c>
+      <c r="K5">
+        <v>75.2</v>
+      </c>
+      <c r="L5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>82.4</v>
+      </c>
+      <c r="C6">
+        <v>40.800000000000004</v>
+      </c>
+      <c r="D6">
+        <v>23.680000000000003</v>
+      </c>
+      <c r="E6">
+        <v>80.800000000000011</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>56.400000000000006</v>
+      </c>
+      <c r="H6">
+        <v>32.04</v>
+      </c>
+      <c r="I6">
+        <v>91.2</v>
+      </c>
+      <c r="J6">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="K6">
+        <v>24.040000000000003</v>
+      </c>
+      <c r="L6">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>64</v>
+      </c>
+      <c r="B7">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="C7">
+        <v>83.2</v>
+      </c>
+      <c r="D7">
+        <v>77.2</v>
+      </c>
+      <c r="E7">
+        <v>25.84</v>
+      </c>
+      <c r="F7">
+        <v>56.400000000000006</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>39.360000000000007</v>
+      </c>
+      <c r="I7">
+        <v>129.6</v>
+      </c>
+      <c r="J7">
+        <v>130.4</v>
+      </c>
+      <c r="K7">
+        <v>63.2</v>
+      </c>
+      <c r="L7">
+        <v>36.800000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>39.760000000000005</v>
+      </c>
+      <c r="B8">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>45.2</v>
+      </c>
+      <c r="D8">
+        <v>45.2</v>
+      </c>
+      <c r="E8">
+        <v>51.2</v>
+      </c>
+      <c r="F8">
+        <v>32.04</v>
+      </c>
+      <c r="G8">
+        <v>39.360000000000007</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>95.2</v>
+      </c>
+      <c r="J8">
+        <v>92.800000000000011</v>
+      </c>
+      <c r="K8">
+        <v>25.64</v>
+      </c>
+      <c r="L8">
+        <v>20.560000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>63.6</v>
+      </c>
+      <c r="B9">
+        <v>122.80000000000001</v>
+      </c>
+      <c r="C9">
+        <v>50.400000000000006</v>
+      </c>
+      <c r="D9">
+        <v>92.4</v>
+      </c>
+      <c r="E9">
+        <v>134.4</v>
+      </c>
+      <c r="F9">
+        <v>91.2</v>
+      </c>
+      <c r="G9">
+        <v>129.6</v>
+      </c>
+      <c r="H9">
+        <v>95.2</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>74.8</v>
+      </c>
+      <c r="K9">
+        <v>72</v>
+      </c>
+      <c r="L9">
+        <v>92.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>84</v>
+      </c>
+      <c r="B10">
+        <v>132.4</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>45.6</v>
+      </c>
+      <c r="E10">
+        <v>142</v>
+      </c>
+      <c r="F10">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="G10">
+        <v>130.4</v>
+      </c>
+      <c r="H10">
+        <v>92.800000000000011</v>
+      </c>
+      <c r="I10">
+        <v>74.8</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>68</v>
+      </c>
+      <c r="L10">
+        <v>100.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>26.04</v>
+      </c>
+      <c r="B11">
+        <v>66</v>
+      </c>
+      <c r="C11">
+        <v>22.400000000000002</v>
+      </c>
+      <c r="D11">
+        <v>27.680000000000003</v>
+      </c>
+      <c r="E11">
+        <v>75.2</v>
+      </c>
+      <c r="F11">
+        <v>24.040000000000003</v>
+      </c>
+      <c r="G11">
+        <v>63.2</v>
+      </c>
+      <c r="H11">
+        <v>25.240000000000002</v>
+      </c>
+      <c r="I11">
+        <v>72</v>
+      </c>
+      <c r="J11">
+        <v>68</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>35.92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>27.400000000000002</v>
+      </c>
+      <c r="B12">
+        <v>30.200000000000003</v>
+      </c>
+      <c r="C12">
+        <v>51.6</v>
+      </c>
+      <c r="D12">
+        <v>61.6</v>
+      </c>
+      <c r="E12">
+        <v>42</v>
+      </c>
+      <c r="F12">
+        <v>53.2</v>
+      </c>
+      <c r="G12">
+        <v>36.800000000000004</v>
+      </c>
+      <c r="H12">
+        <v>20.560000000000002</v>
+      </c>
+      <c r="I12">
+        <v>92.4</v>
+      </c>
+      <c r="J12">
+        <v>100.4</v>
+      </c>
+      <c r="K12">
+        <v>35.92</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="20.875" customWidth="1"/>
-    <col min="4" max="4" width="17.25" customWidth="1"/>
-    <col min="5" max="5" width="15.75" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="5" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1351,187 +1825,187 @@
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>0.2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>1000</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>100</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="5">
         <v>1E-4</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="5">
         <v>10</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixt out of bounds error, excel table voor distances moest een regel lager
</commit_message>
<xml_diff>
--- a/testees.xlsx
+++ b/testees.xlsx
@@ -17,7 +17,7 @@
     <sheet name="distancetable" sheetId="6" r:id="rId3"/>
     <sheet name="Costs" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1307,467 +1307,467 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A2:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>57.6</v>
-      </c>
-      <c r="C1">
-        <v>25.760000000000005</v>
-      </c>
-      <c r="D1">
-        <v>47.6</v>
-      </c>
-      <c r="E1">
-        <v>70</v>
-      </c>
-      <c r="F1">
-        <v>46</v>
-      </c>
-      <c r="G1">
-        <v>64</v>
-      </c>
-      <c r="H1">
-        <v>39.760000000000005</v>
-      </c>
-      <c r="I1">
-        <v>63.6</v>
-      </c>
-      <c r="J1">
-        <v>84</v>
-      </c>
-      <c r="K1">
-        <v>26.04</v>
-      </c>
-      <c r="L1">
-        <v>27.400000000000002</v>
-      </c>
-    </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>57.6</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
       <c r="C2">
-        <v>81.600000000000009</v>
+        <v>25.760000000000005</v>
       </c>
       <c r="D2">
-        <v>91.2</v>
+        <v>47.6</v>
       </c>
       <c r="E2">
-        <v>12.440000000000001</v>
+        <v>70</v>
       </c>
       <c r="F2">
-        <v>82.4</v>
+        <v>46</v>
       </c>
       <c r="G2">
-        <v>32.880000000000003</v>
+        <v>64</v>
       </c>
       <c r="H2">
-        <v>50</v>
+        <v>39.760000000000005</v>
       </c>
       <c r="I2">
-        <v>122.80000000000001</v>
+        <v>63.6</v>
       </c>
       <c r="J2">
-        <v>132.4</v>
+        <v>84</v>
       </c>
       <c r="K2">
-        <v>66</v>
+        <v>26.04</v>
       </c>
       <c r="L2">
-        <v>30.200000000000003</v>
+        <v>27.400000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>25.760000000000005</v>
+        <v>57.6</v>
       </c>
       <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>81.600000000000009</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
       <c r="D3">
-        <v>42.800000000000004</v>
+        <v>91.2</v>
       </c>
       <c r="E3">
-        <v>94.4</v>
+        <v>12.440000000000001</v>
       </c>
       <c r="F3">
-        <v>40.800000000000004</v>
+        <v>82.4</v>
       </c>
       <c r="G3">
-        <v>83.2</v>
+        <v>32.880000000000003</v>
       </c>
       <c r="H3">
-        <v>45.2</v>
+        <v>50</v>
       </c>
       <c r="I3">
-        <v>50.400000000000006</v>
+        <v>122.80000000000001</v>
       </c>
       <c r="J3">
-        <v>60</v>
+        <v>132.4</v>
       </c>
       <c r="K3">
-        <v>22.400000000000002</v>
+        <v>66</v>
       </c>
       <c r="L3">
-        <v>51.6</v>
+        <v>30.200000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>47.6</v>
+        <v>25.760000000000005</v>
       </c>
       <c r="B4">
-        <v>91.2</v>
+        <v>81.600000000000009</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>42.800000000000004</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
       </c>
       <c r="E4">
         <v>94.4</v>
       </c>
       <c r="F4">
-        <v>23.680000000000003</v>
+        <v>40.800000000000004</v>
       </c>
       <c r="G4">
-        <v>77.2</v>
+        <v>83.2</v>
       </c>
       <c r="H4">
         <v>45.2</v>
       </c>
       <c r="I4">
-        <v>92.4</v>
+        <v>50.400000000000006</v>
       </c>
       <c r="J4">
-        <v>45.6</v>
+        <v>60</v>
       </c>
       <c r="K4">
-        <v>27.680000000000003</v>
+        <v>22.400000000000002</v>
       </c>
       <c r="L4">
-        <v>61.6</v>
+        <v>51.6</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>70</v>
+        <v>47.6</v>
       </c>
       <c r="B5">
-        <v>12.440000000000001</v>
+        <v>91.2</v>
       </c>
       <c r="C5">
+        <v>42.800000000000004</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>94.4</v>
       </c>
-      <c r="D5">
-        <v>94.4</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
       <c r="F5">
-        <v>80.800000000000011</v>
+        <v>23.680000000000003</v>
       </c>
       <c r="G5">
-        <v>25.84</v>
+        <v>77.2</v>
       </c>
       <c r="H5">
-        <v>51.2</v>
+        <v>45.2</v>
       </c>
       <c r="I5">
-        <v>134.4</v>
+        <v>92.4</v>
       </c>
       <c r="J5">
-        <v>142</v>
+        <v>45.6</v>
       </c>
       <c r="K5">
-        <v>75.2</v>
+        <v>27.680000000000003</v>
       </c>
       <c r="L5">
-        <v>42</v>
+        <v>61.6</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B6">
-        <v>82.4</v>
+        <v>12.440000000000001</v>
       </c>
       <c r="C6">
-        <v>40.800000000000004</v>
+        <v>94.4</v>
       </c>
       <c r="D6">
-        <v>23.680000000000003</v>
+        <v>94.4</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>80.800000000000011</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
       <c r="G6">
-        <v>56.400000000000006</v>
+        <v>25.84</v>
       </c>
       <c r="H6">
-        <v>32.04</v>
+        <v>51.2</v>
       </c>
       <c r="I6">
-        <v>91.2</v>
+        <v>134.4</v>
       </c>
       <c r="J6">
-        <v>66.400000000000006</v>
+        <v>142</v>
       </c>
       <c r="K6">
-        <v>24.040000000000003</v>
+        <v>75.2</v>
       </c>
       <c r="L6">
-        <v>53.2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B7">
-        <v>32.880000000000003</v>
+        <v>82.4</v>
       </c>
       <c r="C7">
-        <v>83.2</v>
+        <v>40.800000000000004</v>
       </c>
       <c r="D7">
-        <v>77.2</v>
+        <v>23.680000000000003</v>
       </c>
       <c r="E7">
-        <v>25.84</v>
+        <v>80.800000000000011</v>
       </c>
       <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>56.400000000000006</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
       <c r="H7">
-        <v>39.360000000000007</v>
+        <v>32.04</v>
       </c>
       <c r="I7">
-        <v>129.6</v>
+        <v>91.2</v>
       </c>
       <c r="J7">
-        <v>130.4</v>
+        <v>66.400000000000006</v>
       </c>
       <c r="K7">
-        <v>63.2</v>
+        <v>24.040000000000003</v>
       </c>
       <c r="L7">
-        <v>36.800000000000004</v>
+        <v>53.2</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>39.760000000000005</v>
+        <v>64</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>32.880000000000003</v>
       </c>
       <c r="C8">
-        <v>45.2</v>
+        <v>83.2</v>
       </c>
       <c r="D8">
-        <v>45.2</v>
+        <v>77.2</v>
       </c>
       <c r="E8">
-        <v>51.2</v>
+        <v>25.84</v>
       </c>
       <c r="F8">
-        <v>32.04</v>
+        <v>56.400000000000006</v>
       </c>
       <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>39.360000000000007</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
       <c r="I8">
-        <v>95.2</v>
+        <v>129.6</v>
       </c>
       <c r="J8">
-        <v>92.800000000000011</v>
+        <v>130.4</v>
       </c>
       <c r="K8">
-        <v>25.64</v>
+        <v>63.2</v>
       </c>
       <c r="L8">
-        <v>20.560000000000002</v>
+        <v>36.800000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>63.6</v>
+        <v>39.760000000000005</v>
       </c>
       <c r="B9">
-        <v>122.80000000000001</v>
+        <v>50</v>
       </c>
       <c r="C9">
-        <v>50.400000000000006</v>
+        <v>45.2</v>
       </c>
       <c r="D9">
-        <v>92.4</v>
+        <v>45.2</v>
       </c>
       <c r="E9">
-        <v>134.4</v>
+        <v>51.2</v>
       </c>
       <c r="F9">
-        <v>91.2</v>
+        <v>32.04</v>
       </c>
       <c r="G9">
-        <v>129.6</v>
+        <v>39.360000000000007</v>
       </c>
       <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>95.2</v>
       </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
       <c r="J9">
-        <v>74.8</v>
+        <v>92.800000000000011</v>
       </c>
       <c r="K9">
-        <v>72</v>
+        <v>25.64</v>
       </c>
       <c r="L9">
-        <v>92.4</v>
+        <v>20.560000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>84</v>
+        <v>63.6</v>
       </c>
       <c r="B10">
-        <v>132.4</v>
+        <v>122.80000000000001</v>
       </c>
       <c r="C10">
-        <v>60</v>
+        <v>50.400000000000006</v>
       </c>
       <c r="D10">
-        <v>45.6</v>
+        <v>92.4</v>
       </c>
       <c r="E10">
-        <v>142</v>
+        <v>134.4</v>
       </c>
       <c r="F10">
-        <v>66.400000000000006</v>
+        <v>91.2</v>
       </c>
       <c r="G10">
-        <v>130.4</v>
+        <v>129.6</v>
       </c>
       <c r="H10">
-        <v>92.800000000000011</v>
+        <v>95.2</v>
       </c>
       <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
         <v>74.8</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
       <c r="K10">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="L10">
-        <v>100.4</v>
+        <v>92.4</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>26.04</v>
+        <v>84</v>
       </c>
       <c r="B11">
-        <v>66</v>
+        <v>132.4</v>
       </c>
       <c r="C11">
-        <v>22.400000000000002</v>
+        <v>60</v>
       </c>
       <c r="D11">
-        <v>27.680000000000003</v>
+        <v>45.6</v>
       </c>
       <c r="E11">
-        <v>75.2</v>
+        <v>142</v>
       </c>
       <c r="F11">
-        <v>24.040000000000003</v>
+        <v>66.400000000000006</v>
       </c>
       <c r="G11">
-        <v>63.2</v>
+        <v>130.4</v>
       </c>
       <c r="H11">
-        <v>25.240000000000002</v>
+        <v>92.800000000000011</v>
       </c>
       <c r="I11">
-        <v>72</v>
+        <v>74.8</v>
       </c>
       <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
         <v>68</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
       <c r="L11">
-        <v>35.92</v>
+        <v>100.4</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>26.04</v>
+      </c>
+      <c r="B12">
+        <v>66</v>
+      </c>
+      <c r="C12">
+        <v>22.400000000000002</v>
+      </c>
+      <c r="D12">
+        <v>27.680000000000003</v>
+      </c>
+      <c r="E12">
+        <v>75.2</v>
+      </c>
+      <c r="F12">
+        <v>24.040000000000003</v>
+      </c>
+      <c r="G12">
+        <v>63.2</v>
+      </c>
+      <c r="H12">
+        <v>25.240000000000002</v>
+      </c>
+      <c r="I12">
+        <v>72</v>
+      </c>
+      <c r="J12">
+        <v>68</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>35.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>27.400000000000002</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>30.200000000000003</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>51.6</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>61.6</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>42</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>53.2</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>36.800000000000004</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>20.560000000000002</v>
       </c>
-      <c r="I12">
+      <c r="I13">
         <v>92.4</v>
       </c>
-      <c r="J12">
+      <c r="J13">
         <v>100.4</v>
       </c>
-      <c r="K12">
+      <c r="K13">
         <v>35.92</v>
       </c>
-      <c r="L12">
+      <c r="L13">
         <v>0</v>
       </c>
     </row>
@@ -1971,41 +1971,41 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added random pool of testees to excel
</commit_message>
<xml_diff>
--- a/testees.xlsx
+++ b/testees.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26124"/>
-  <workbookPr showInkAnnotation="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liesbethwijn/PycharmProjects/Operations_JoshLiesErik/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikvanbaasbank\PycharmProjects\Operations_JoshLiesErik\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB66CC3-FE0F-4776-905E-8B6EC97B1CA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RandomPopulation" sheetId="1" r:id="rId1"/>
@@ -17,11 +18,8 @@
     <sheet name="distancetable" sheetId="6" r:id="rId3"/>
     <sheet name="Costs" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -31,12 +29,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>timepref</t>
   </si>
@@ -171,12 +172,15 @@
   </si>
   <si>
     <t>LL</t>
+  </si>
+  <si>
+    <t>Occurances in final sheet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -262,22 +266,33 @@
     </xf>
   </cellXfs>
   <cellStyles count="14">
-    <cellStyle name="Comma 2" xfId="2"/>
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Procent 2" xfId="4"/>
-    <cellStyle name="Standaard 2" xfId="3"/>
-    <cellStyle name="Standaard 2 2" xfId="12"/>
-    <cellStyle name="Standaard 3" xfId="5"/>
-    <cellStyle name="Standaard 4" xfId="13"/>
-    <cellStyle name="Standaard_Blad1" xfId="11"/>
-    <cellStyle name="style1499936711542" xfId="6"/>
-    <cellStyle name="style1499936711557" xfId="7"/>
-    <cellStyle name="style1499936711635" xfId="8"/>
-    <cellStyle name="style1499936711651" xfId="9"/>
-    <cellStyle name="style1499936712276" xfId="10"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Procent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Standaard 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Standaard 2 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Standaard 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Standaard 4" xfId="13" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Standaard_Blad1" xfId="11" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="style1499936711542" xfId="6" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="style1499936711557" xfId="7" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="style1499936711635" xfId="8" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="style1499936711651" xfId="9" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="style1499936712276" xfId="10" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -552,14 +567,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:B203"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A25"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -574,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -582,12 +598,12 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -595,7 +611,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -603,34 +619,34 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -643,7 +659,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -654,7 +670,7 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -662,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -670,82 +686,82 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -753,71 +769,71 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
       <c r="B26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
       <c r="B28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
       <c r="B30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -825,15 +841,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
       <c r="B34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -841,25 +857,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
       <c r="B36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -867,208 +883,1356 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B45">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B46">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B50">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
     </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>6</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>6</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>6</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>6</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>6</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>6</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>6</v>
+      </c>
+      <c r="B67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>6</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>6</v>
+      </c>
+      <c r="B69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>6</v>
+      </c>
+      <c r="B70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>7</v>
+      </c>
+      <c r="B71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>7</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>7</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>7</v>
+      </c>
+      <c r="B74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>7</v>
+      </c>
+      <c r="B75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>7</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>7</v>
+      </c>
+      <c r="B77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>7</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>7</v>
+      </c>
+      <c r="B79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>7</v>
+      </c>
+      <c r="B80">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>7</v>
+      </c>
+      <c r="B81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>7</v>
+      </c>
+      <c r="B82">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>7</v>
+      </c>
+      <c r="B83">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>7</v>
+      </c>
+      <c r="B84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>7</v>
+      </c>
+      <c r="B85">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>7</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>7</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>7</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>7</v>
+      </c>
+      <c r="B89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>7</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>7</v>
+      </c>
+      <c r="B91">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>7</v>
+      </c>
+      <c r="B92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>7</v>
+      </c>
+      <c r="B93">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>7</v>
+      </c>
+      <c r="B94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>7</v>
+      </c>
+      <c r="B95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>7</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>7</v>
+      </c>
+      <c r="B97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>7</v>
+      </c>
+      <c r="B98">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>7</v>
+      </c>
+      <c r="B99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>7</v>
+      </c>
+      <c r="B100">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>7</v>
+      </c>
+      <c r="B101">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>7</v>
+      </c>
+      <c r="B102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>7</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>7</v>
+      </c>
+      <c r="B104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>7</v>
+      </c>
+      <c r="B105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>8</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>8</v>
+      </c>
+      <c r="B107">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>8</v>
+      </c>
+      <c r="B108">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>8</v>
+      </c>
+      <c r="B109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>8</v>
+      </c>
+      <c r="B110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>8</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>8</v>
+      </c>
+      <c r="B112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>8</v>
+      </c>
+      <c r="B113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>8</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>8</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>8</v>
+      </c>
+      <c r="B116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>8</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>8</v>
+      </c>
+      <c r="B118">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>8</v>
+      </c>
+      <c r="B119">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>8</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>8</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>8</v>
+      </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>8</v>
+      </c>
+      <c r="B123">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>8</v>
+      </c>
+      <c r="B124">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>8</v>
+      </c>
+      <c r="B125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>8</v>
+      </c>
+      <c r="B126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>8</v>
+      </c>
+      <c r="B127">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>8</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>8</v>
+      </c>
+      <c r="B129">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>8</v>
+      </c>
+      <c r="B130">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>8</v>
+      </c>
+      <c r="B131">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>8</v>
+      </c>
+      <c r="B132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>8</v>
+      </c>
+      <c r="B133">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>8</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>8</v>
+      </c>
+      <c r="B135">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>8</v>
+      </c>
+      <c r="B136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>8</v>
+      </c>
+      <c r="B137">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>8</v>
+      </c>
+      <c r="B138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>8</v>
+      </c>
+      <c r="B139">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>8</v>
+      </c>
+      <c r="B140">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>8</v>
+      </c>
+      <c r="B141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>8</v>
+      </c>
+      <c r="B142">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>8</v>
+      </c>
+      <c r="B143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>8</v>
+      </c>
+      <c r="B144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>8</v>
+      </c>
+      <c r="B145">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>8</v>
+      </c>
+      <c r="B146">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>8</v>
+      </c>
+      <c r="B147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>8</v>
+      </c>
+      <c r="B148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>8</v>
+      </c>
+      <c r="B149">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>8</v>
+      </c>
+      <c r="B150">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>8</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>8</v>
+      </c>
+      <c r="B152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>8</v>
+      </c>
+      <c r="B153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>8</v>
+      </c>
+      <c r="B154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>8</v>
+      </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>8</v>
+      </c>
+      <c r="B156">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>8</v>
+      </c>
+      <c r="B157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>8</v>
+      </c>
+      <c r="B158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>9</v>
+      </c>
+      <c r="B159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>9</v>
+      </c>
+      <c r="B160">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>9</v>
+      </c>
+      <c r="B161">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>9</v>
+      </c>
+      <c r="B162">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>9</v>
+      </c>
+      <c r="B163">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>9</v>
+      </c>
+      <c r="B164">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>9</v>
+      </c>
+      <c r="B165">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>9</v>
+      </c>
+      <c r="B166">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>9</v>
+      </c>
+      <c r="B167">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>9</v>
+      </c>
+      <c r="B168">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>9</v>
+      </c>
+      <c r="B169">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>9</v>
+      </c>
+      <c r="B170">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>9</v>
+      </c>
+      <c r="B171">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>9</v>
+      </c>
+      <c r="B172">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>9</v>
+      </c>
+      <c r="B173">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>10</v>
+      </c>
+      <c r="B174">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>10</v>
+      </c>
+      <c r="B175">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>10</v>
+      </c>
+      <c r="B176">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>10</v>
+      </c>
+      <c r="B177">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>10</v>
+      </c>
+      <c r="B178">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>10</v>
+      </c>
+      <c r="B179">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>10</v>
+      </c>
+      <c r="B180">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>10</v>
+      </c>
+      <c r="B181">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>10</v>
+      </c>
+      <c r="B182">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>10</v>
+      </c>
+      <c r="B183">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>10</v>
+      </c>
+      <c r="B184">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>10</v>
+      </c>
+      <c r="B185">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>10</v>
+      </c>
+      <c r="B186">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>10</v>
+      </c>
+      <c r="B187">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>11</v>
+      </c>
+      <c r="B188">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>11</v>
+      </c>
+      <c r="B189">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>11</v>
+      </c>
+      <c r="B190">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>11</v>
+      </c>
+      <c r="B191">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>12</v>
+      </c>
+      <c r="B192">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>12</v>
+      </c>
+      <c r="B193">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>12</v>
+      </c>
+      <c r="B194">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>12</v>
+      </c>
+      <c r="B195">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>12</v>
+      </c>
+      <c r="B196">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>12</v>
+      </c>
+      <c r="B197">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>12</v>
+      </c>
+      <c r="B198">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>12</v>
+      </c>
+      <c r="B199">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>12</v>
+      </c>
+      <c r="B200">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>12</v>
+      </c>
+      <c r="B201">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>12</v>
+      </c>
+      <c r="B202">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>12</v>
+      </c>
+      <c r="B203">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B60">
+    <sortCondition ref="A1:A60"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="5" max="5" width="7.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>40</v>
@@ -1076,222 +2240,272 @@
       <c r="E1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" t="s">
         <v>29</v>
       </c>
+      <c r="B2">
+        <v>202000</v>
+      </c>
       <c r="C2">
-        <v>202000</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C2)</f>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B2)</f>
         <v>20</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
+      <c r="F2">
+        <f>COUNTIF(RandomPopulation!$A:$A,C2)</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
+      <c r="B3">
+        <v>96000</v>
+      </c>
       <c r="C3">
-        <v>96000</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C3)</f>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B3)</f>
         <v>9</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
+      <c r="F3">
+        <f>COUNTIF(RandomPopulation!$A:$A,C3)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" t="s">
         <v>31</v>
       </c>
+      <c r="B4">
+        <v>67000</v>
+      </c>
       <c r="C4">
-        <v>67000</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C4)</f>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B4)</f>
         <v>6</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
+      <c r="F4">
+        <f>COUNTIF(RandomPopulation!$A:$A,C4)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" t="s">
         <v>37</v>
       </c>
+      <c r="B5">
+        <v>76000</v>
+      </c>
       <c r="C5">
-        <v>76000</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C5)</f>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B5)</f>
         <v>7</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
+      <c r="F5">
+        <f>COUNTIF(RandomPopulation!$A:$A,C5)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" t="s">
         <v>32</v>
       </c>
+      <c r="B6">
+        <v>123000</v>
+      </c>
       <c r="C6">
-        <v>123000</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C6)</f>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B6)</f>
         <v>12</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
+      <c r="F6">
+        <f>COUNTIF(RandomPopulation!$A:$A,C6)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>154000</v>
+      </c>
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7">
-        <v>154000</v>
-      </c>
       <c r="D7">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C7)</f>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B7)</f>
         <v>15</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
+      <c r="F7">
+        <f>COUNTIF(RandomPopulation!$A:$A,C7)</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>353000</v>
       </c>
       <c r="C8">
-        <v>353000</v>
+        <v>7</v>
       </c>
       <c r="D8">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C8)</f>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B8)</f>
         <v>35</v>
       </c>
       <c r="E8">
         <v>10</v>
       </c>
+      <c r="F8">
+        <f>COUNTIF(RandomPopulation!$A:$A,C8)</f>
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="A9" t="s">
         <v>38</v>
       </c>
+      <c r="B9">
+        <v>538000</v>
+      </c>
       <c r="C9">
-        <v>538000</v>
+        <v>8</v>
       </c>
       <c r="D9">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C9)</f>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B9)</f>
         <v>53</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
+      <c r="F9">
+        <f>COUNTIF(RandomPopulation!$A:$A,C9)</f>
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10">
+        <v>150000</v>
+      </c>
+      <c r="C10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10">
-        <v>150000</v>
-      </c>
       <c r="D10">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C10)</f>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B10)</f>
         <v>15</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
+      <c r="F10">
+        <f>COUNTIF(RandomPopulation!$A:$A,C10)</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <v>143000</v>
+      </c>
+      <c r="C11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11">
-        <v>143000</v>
-      </c>
       <c r="D11">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C11)</f>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B11)</f>
         <v>14</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
+      <c r="F11">
+        <f>COUNTIF(RandomPopulation!$A:$A,C11)</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>47700</v>
+      </c>
+      <c r="C12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12">
-        <v>47700</v>
-      </c>
       <c r="D12">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C12)</f>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B12)</f>
         <v>4</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
+      <c r="F12">
+        <f>COUNTIF(RandomPopulation!$A:$A,C12)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <v>121000</v>
+      </c>
+      <c r="C13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13">
-        <v>121000</v>
-      </c>
       <c r="D13">
-        <f>_xlfn.FLOOR.MATH(Costs!$C$10*C13)</f>
+        <f>_xlfn.FLOOR.MATH(Costs!$C$10*B13)</f>
         <v>12</v>
       </c>
       <c r="E13">
         <v>10</v>
+      </c>
+      <c r="F13">
+        <f>COUNTIF(RandomPopulation!$A:$A,C13)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1299,23 +2513,33 @@
         <f>SUM(D2:D13)</f>
         <v>202</v>
       </c>
+      <c r="F14">
+        <f>SUM(F2:F13)</f>
+        <v>202</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F14">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>$D$14</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1353,7 +2577,7 @@
         <v>27.400000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>57.6</v>
       </c>
@@ -1391,7 +2615,7 @@
         <v>30.200000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>25.760000000000005</v>
       </c>
@@ -1429,7 +2653,7 @@
         <v>51.6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>47.6</v>
       </c>
@@ -1467,7 +2691,7 @@
         <v>61.6</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>70</v>
       </c>
@@ -1505,7 +2729,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>46</v>
       </c>
@@ -1543,7 +2767,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>64</v>
       </c>
@@ -1581,7 +2805,7 @@
         <v>36.800000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>39.760000000000005</v>
       </c>
@@ -1619,7 +2843,7 @@
         <v>20.560000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>63.6</v>
       </c>
@@ -1657,7 +2881,7 @@
         <v>92.4</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>84</v>
       </c>
@@ -1695,7 +2919,7 @@
         <v>100.4</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>26.04</v>
       </c>
@@ -1733,7 +2957,7 @@
         <v>35.92</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>27.400000000000002</v>
       </c>
@@ -1777,23 +3001,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.875" customWidth="1"/>
+    <col min="4" max="4" width="17.125" customWidth="1"/>
+    <col min="5" max="5" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
         <v>3</v>
@@ -1809,7 +3034,7 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1817,7 +3042,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1825,7 +3050,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -1843,7 +3068,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1851,7 +3076,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1869,7 +3094,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1877,7 +3102,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1895,7 +3120,7 @@
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1903,7 +3128,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -1918,14 +3143,14 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
@@ -1940,14 +3165,14 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
@@ -1962,7 +3187,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1971,41 +3196,41 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated capacity, costs, and prints
</commit_message>
<xml_diff>
--- a/testees.xlsx
+++ b/testees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikvanbaasbank\PycharmProjects\Operations_JoshLiesErik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96019FA-3A04-4BF9-B90B-4B6E1A436D2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741C9E4C-B26B-4D84-B0F5-6C8F00739299}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="78">
   <si>
     <t>timepref</t>
   </si>
@@ -57,9 +79,6 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -87,15 +106,6 @@
     <t>€ / TK</t>
   </si>
   <si>
-    <t>Average travel reimbursement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Includes hourly wage of five coworkers per street and location </t>
-  </si>
-  <si>
-    <t>Based off of fast-test</t>
-  </si>
-  <si>
     <t>Nr of testees per city</t>
   </si>
   <si>
@@ -180,22 +190,109 @@
     <t>Cost per 2-lane corona street</t>
   </si>
   <si>
-    <t>Firemen for logistics</t>
-  </si>
-  <si>
-    <t>Students for testing and administration</t>
-  </si>
-  <si>
-    <t>Coordinators</t>
-  </si>
-  <si>
     <t>Working hours 9-17</t>
   </si>
   <si>
-    <t>Total cost</t>
-  </si>
-  <si>
-    <t>Cost per employees</t>
+    <t>Total cost per test site</t>
+  </si>
+  <si>
+    <t>eu/h</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Average inhabitants per city</t>
+  </si>
+  <si>
+    <t>Capacity required if two cities close down</t>
+  </si>
+  <si>
+    <t>Total testees</t>
+  </si>
+  <si>
+    <t>Total cities</t>
+  </si>
+  <si>
+    <t>Max nr test locations closed down</t>
+  </si>
+  <si>
+    <t>Average cost per employee</t>
+  </si>
+  <si>
+    <t>Travel kost per kilometer</t>
+  </si>
+  <si>
+    <t>Travel cost per kilometer ov</t>
+  </si>
+  <si>
+    <t>Cleartest</t>
+  </si>
+  <si>
+    <t>Estimated cost for government</t>
+  </si>
+  <si>
+    <t>https://www.medischevakhandel.nl/nl/sneltest-corona-virus-coronatest.html</t>
+  </si>
+  <si>
+    <t>Heagen</t>
+  </si>
+  <si>
+    <t>Commercial test kits</t>
+  </si>
+  <si>
+    <t>https://www.arbowinkel.nl/corona-sneltest-covid-19-igg-igm-test.html</t>
+  </si>
+  <si>
+    <t>Abbott</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>https://www.bhvtotaal.nl/abbott-corona-sneltest</t>
+  </si>
+  <si>
+    <t>Government voordee factor ???</t>
+  </si>
+  <si>
+    <t>eu/km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selected </t>
+  </si>
+  <si>
+    <t>Capcity per week</t>
+  </si>
+  <si>
+    <t>Amount of timeslots in a week</t>
+  </si>
+  <si>
+    <t>Test capacity per day</t>
+  </si>
+  <si>
+    <t>Test capacity per week</t>
+  </si>
+  <si>
+    <t>Weekly capacity reqif two cities close down</t>
+  </si>
+  <si>
+    <t>Nr. firemen for logistics</t>
+  </si>
+  <si>
+    <t>Nr. students for testing and administration</t>
+  </si>
+  <si>
+    <t>Nr. coordinators</t>
+  </si>
+  <si>
+    <t>Constants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -205,9 +302,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -233,13 +337,51 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -251,42 +393,87 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="14"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="14" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="17"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="17" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="16"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="16" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="16" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="15"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="15" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="12"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="14" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="16" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="16" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="15" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="15" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="18"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="18" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="18" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="19">
+    <cellStyle name="20% - Accent1" xfId="14" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="15" builtinId="34"/>
+    <cellStyle name="20% - Accent3" xfId="16" builtinId="38"/>
+    <cellStyle name="20% - Accent4" xfId="17" builtinId="42"/>
+    <cellStyle name="20% - Accent6" xfId="18" builtinId="50"/>
     <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -593,7 +780,7 @@
   <dimension ref="A1:B203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F124" sqref="F124"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2236,7 +2423,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2247,28 +2434,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>202000</v>
@@ -2290,7 +2477,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>96000</v>
@@ -2312,7 +2499,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>67000</v>
@@ -2334,7 +2521,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>76000</v>
@@ -2356,7 +2543,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>123000</v>
@@ -2378,7 +2565,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>154000</v>
@@ -2422,7 +2609,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>538000</v>
@@ -2444,7 +2631,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B10">
         <v>150000</v>
@@ -2466,7 +2653,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B11">
         <v>143000</v>
@@ -2488,7 +2675,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B12">
         <v>47700</v>
@@ -2510,7 +2697,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B13">
         <v>121000</v>
@@ -3025,279 +3212,487 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="20.875" customWidth="1"/>
-    <col min="4" max="4" width="17.125" customWidth="1"/>
-    <col min="5" max="5" width="15.625" customWidth="1"/>
-    <col min="11" max="11" width="27.375" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="12" customWidth="1"/>
+    <col min="2" max="2" width="29.25" style="12" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="12" customWidth="1"/>
+    <col min="4" max="4" width="13" style="12" customWidth="1"/>
+    <col min="10" max="10" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="J1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="1"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="K1" s="3" t="s">
+      <c r="B3" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="23">
+        <f>K31</f>
+        <v>0.2</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="4">
+        <v>16</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="21">
+        <f>K9</f>
+        <v>1664</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="4">
+        <v>6</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="25">
+        <f>K40</f>
+        <v>100</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K5" s="4">
+        <v>6</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="28">
+        <f>K25</f>
+        <v>5</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="J6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="4">
+        <v>8</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="5">
+        <f>K3*(K4+K5+K6)*K7</f>
+        <v>1664</v>
+      </c>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="7"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="6">
+        <v>12</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" s="6">
+        <f>StedenInformatie!$D$14</f>
+        <v>202</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="6">
+        <f>ROUNDUP(AVERAGE(StedenInformatie!$D$2:$D$13),0)</f>
+        <v>17</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="J16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" s="6">
+        <v>2</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J18" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K18" s="7">
+        <f>ROUNDUP(K14/(K13-K16),0)</f>
+        <v>21</v>
+      </c>
+      <c r="L18" s="6"/>
+    </row>
+    <row r="20" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J20" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="K20" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="L20" s="26"/>
+    </row>
+    <row r="21" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+    </row>
+    <row r="22" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J22" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="K22" s="26">
+        <f>K18</f>
+        <v>21</v>
+      </c>
+      <c r="L22" s="26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J23" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="K23" s="26">
+        <v>5</v>
+      </c>
+      <c r="L23" s="26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+    </row>
+    <row r="25" spans="10:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="K25" s="27">
+        <f>ROUNDUP(K22/K23,0)</f>
+        <v>5</v>
+      </c>
+      <c r="L25" s="26"/>
+    </row>
+    <row r="26" spans="10:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="10:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27" s="9"/>
+    </row>
+    <row r="28" spans="10:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+    </row>
+    <row r="29" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J29" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K29" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="L29" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+    </row>
+    <row r="31" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J31" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K31" s="13">
         <v>0.2</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="K4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="2"/>
-      <c r="K5" t="s">
-        <v>47</v>
-      </c>
-      <c r="L5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1000</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="K6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="2"/>
-      <c r="K7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="L31" s="8"/>
+    </row>
+    <row r="33" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J33" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="K33" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="L33" s="17"/>
+      <c r="M33" s="20"/>
+    </row>
+    <row r="34" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="20"/>
+    </row>
+    <row r="35" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J35" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K35" s="15">
+        <v>275</v>
+      </c>
+      <c r="L35" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M35" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="N35" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J36" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K36" s="15">
+        <v>250</v>
+      </c>
+      <c r="L36" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M36" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="N36" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K37" s="15">
+        <v>225</v>
+      </c>
+      <c r="L37" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M37" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N37" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J38" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="K38" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="M38" s="20"/>
+      <c r="N38" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="19"/>
+    </row>
+    <row r="40" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J40" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K40" s="18" cm="1">
+        <f t="array" ref="K40">AVERAGE(K35:K37*K38)</f>
         <v>100</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="K8" t="s">
-        <v>50</v>
-      </c>
-      <c r="L8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="K10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L10" s="3">
-        <f>L4*(L5+L6+L7)*L8</f>
-        <v>1664</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="5">
-        <v>10</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="20"/>
+    </row>
+    <row r="41" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="M41" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Small edit in testees.xlsx
</commit_message>
<xml_diff>
--- a/testees.xlsx
+++ b/testees.xlsx
@@ -5,18 +5,19 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikvanbaasbank\PycharmProjects\Operations_JoshLiesErik\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\PycharmProjects\Operations_JoshLiesErik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959A33FC-B7DB-4828-8AD7-70D7A6E192E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004228EA-3E51-4A49-BD24-F3D7C1FEB0F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RandomPopulation" sheetId="1" r:id="rId1"/>
     <sheet name="StedenInformatie" sheetId="5" r:id="rId2"/>
     <sheet name="distancetable" sheetId="6" r:id="rId3"/>
-    <sheet name="Costs" sheetId="3" r:id="rId4"/>
+    <sheet name="distancetable (2)" sheetId="8" r:id="rId4"/>
+    <sheet name="Costs" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,30 +37,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
   <si>
     <t>timepref</t>
   </si>
@@ -79,6 +58,9 @@
     <t>Unit</t>
   </si>
   <si>
+    <t>Comment</t>
+  </si>
+  <si>
     <t>C1</t>
   </si>
   <si>
@@ -106,6 +88,15 @@
     <t>€ / TK</t>
   </si>
   <si>
+    <t>Average travel reimbursement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes hourly wage of five coworkers per street and location </t>
+  </si>
+  <si>
+    <t>Based off of fast-test</t>
+  </si>
+  <si>
     <t>Nr of testees per city</t>
   </si>
   <si>
@@ -185,117 +176,6 @@
   </si>
   <si>
     <t>Occurances in final sheet</t>
-  </si>
-  <si>
-    <t>Cost per 2-lane corona street</t>
-  </si>
-  <si>
-    <t>Working hours 9-17</t>
-  </si>
-  <si>
-    <t>Total cost per test site</t>
-  </si>
-  <si>
-    <t>eu/h</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>Average inhabitants per city</t>
-  </si>
-  <si>
-    <t>Capacity required if two cities close down</t>
-  </si>
-  <si>
-    <t>Total testees</t>
-  </si>
-  <si>
-    <t>Total cities</t>
-  </si>
-  <si>
-    <t>Max nr test locations closed down</t>
-  </si>
-  <si>
-    <t>Average cost per employee</t>
-  </si>
-  <si>
-    <t>Travel kost per kilometer</t>
-  </si>
-  <si>
-    <t>Travel cost per kilometer ov</t>
-  </si>
-  <si>
-    <t>Cleartest</t>
-  </si>
-  <si>
-    <t>Estimated cost for government</t>
-  </si>
-  <si>
-    <t>https://www.medischevakhandel.nl/nl/sneltest-corona-virus-coronatest.html</t>
-  </si>
-  <si>
-    <t>Heagen</t>
-  </si>
-  <si>
-    <t>Commercial test kits</t>
-  </si>
-  <si>
-    <t>https://www.arbowinkel.nl/corona-sneltest-covid-19-igg-igm-test.html</t>
-  </si>
-  <si>
-    <t>Abbott</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>https://www.bhvtotaal.nl/abbott-corona-sneltest</t>
-  </si>
-  <si>
-    <t>eu/km</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selected </t>
-  </si>
-  <si>
-    <t>Capcity per week</t>
-  </si>
-  <si>
-    <t>Amount of timeslots in a week</t>
-  </si>
-  <si>
-    <t>Test capacity per day</t>
-  </si>
-  <si>
-    <t>Test capacity per week</t>
-  </si>
-  <si>
-    <t>Weekly capacity reqif two cities close down</t>
-  </si>
-  <si>
-    <t>Nr. firemen for logistics</t>
-  </si>
-  <si>
-    <t>Nr. students for testing and administration</t>
-  </si>
-  <si>
-    <t>Nr. coordinators</t>
-  </si>
-  <si>
-    <t>Constants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t>Government voordeel factor ???</t>
-  </si>
-  <si>
-    <t>Selected</t>
   </si>
 </sst>
 </file>
@@ -305,23 +185,9 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -347,51 +213,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -403,91 +231,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="14"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="14" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="17"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="17" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="16"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="16" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="16" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="15"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="15" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="12"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="14" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="16" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="16" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="15" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="15" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="18"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="18" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="18" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
-    <cellStyle name="20% - Accent1" xfId="14" builtinId="30"/>
-    <cellStyle name="20% - Accent2" xfId="15" builtinId="34"/>
-    <cellStyle name="20% - Accent3" xfId="16" builtinId="38"/>
-    <cellStyle name="20% - Accent4" xfId="17" builtinId="42"/>
-    <cellStyle name="20% - Accent6" xfId="18" builtinId="50"/>
+  <cellStyles count="14">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -793,13 +572,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B203"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -807,7 +586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -815,7 +594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -823,7 +602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -831,7 +610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -839,7 +618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -847,7 +626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -855,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -863,7 +642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -871,7 +650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -879,7 +658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -887,7 +666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -895,7 +674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -903,7 +682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -911,7 +690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -919,7 +698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -927,7 +706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -935,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -943,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -951,7 +730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -959,7 +738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -967,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -975,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -983,7 +762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2</v>
       </c>
@@ -991,7 +770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -999,7 +778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1007,7 +786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1015,7 +794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1023,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1031,7 +810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1039,7 +818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1047,7 +826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1055,7 +834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1063,7 +842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1071,7 +850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1079,7 +858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1087,7 +866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4</v>
       </c>
@@ -1095,7 +874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4</v>
       </c>
@@ -1103,7 +882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>4</v>
       </c>
@@ -1111,7 +890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4</v>
       </c>
@@ -1119,7 +898,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1127,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>4</v>
       </c>
@@ -1135,7 +914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>4</v>
       </c>
@@ -1143,7 +922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>5</v>
       </c>
@@ -1151,7 +930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>5</v>
       </c>
@@ -1159,7 +938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>5</v>
       </c>
@@ -1167,7 +946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>5</v>
       </c>
@@ -1175,7 +954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>5</v>
       </c>
@@ -1183,7 +962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>5</v>
       </c>
@@ -1191,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>5</v>
       </c>
@@ -1199,7 +978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>5</v>
       </c>
@@ -1207,7 +986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>5</v>
       </c>
@@ -1215,7 +994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>5</v>
       </c>
@@ -1223,7 +1002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>5</v>
       </c>
@@ -1231,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>5</v>
       </c>
@@ -1239,7 +1018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>6</v>
       </c>
@@ -1247,7 +1026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>6</v>
       </c>
@@ -1255,7 +1034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>6</v>
       </c>
@@ -1263,7 +1042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>6</v>
       </c>
@@ -1271,7 +1050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>6</v>
       </c>
@@ -1279,7 +1058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>6</v>
       </c>
@@ -1287,7 +1066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>6</v>
       </c>
@@ -1295,7 +1074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>6</v>
       </c>
@@ -1303,7 +1082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>6</v>
       </c>
@@ -1311,7 +1090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>6</v>
       </c>
@@ -1319,7 +1098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>6</v>
       </c>
@@ -1327,7 +1106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>6</v>
       </c>
@@ -1335,7 +1114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>6</v>
       </c>
@@ -1343,7 +1122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>6</v>
       </c>
@@ -1351,7 +1130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>6</v>
       </c>
@@ -1359,7 +1138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>7</v>
       </c>
@@ -1367,7 +1146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>7</v>
       </c>
@@ -1375,7 +1154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>7</v>
       </c>
@@ -1383,7 +1162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>7</v>
       </c>
@@ -1391,7 +1170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>7</v>
       </c>
@@ -1399,7 +1178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>7</v>
       </c>
@@ -1407,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>7</v>
       </c>
@@ -1415,7 +1194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>7</v>
       </c>
@@ -1423,7 +1202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>7</v>
       </c>
@@ -1431,7 +1210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>7</v>
       </c>
@@ -1439,7 +1218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>7</v>
       </c>
@@ -1447,7 +1226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>7</v>
       </c>
@@ -1455,7 +1234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>7</v>
       </c>
@@ -1463,7 +1242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>7</v>
       </c>
@@ -1471,7 +1250,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>7</v>
       </c>
@@ -1479,7 +1258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>7</v>
       </c>
@@ -1487,7 +1266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>7</v>
       </c>
@@ -1495,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>7</v>
       </c>
@@ -1503,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>7</v>
       </c>
@@ -1511,7 +1290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>7</v>
       </c>
@@ -1519,7 +1298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>7</v>
       </c>
@@ -1527,7 +1306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>7</v>
       </c>
@@ -1535,7 +1314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>7</v>
       </c>
@@ -1543,7 +1322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>7</v>
       </c>
@@ -1551,7 +1330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>7</v>
       </c>
@@ -1559,7 +1338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>7</v>
       </c>
@@ -1567,7 +1346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>7</v>
       </c>
@@ -1575,7 +1354,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>7</v>
       </c>
@@ -1583,7 +1362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>7</v>
       </c>
@@ -1591,7 +1370,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>7</v>
       </c>
@@ -1599,7 +1378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>7</v>
       </c>
@@ -1607,7 +1386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>7</v>
       </c>
@@ -1615,7 +1394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>7</v>
       </c>
@@ -1623,7 +1402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>7</v>
       </c>
@@ -1631,7 +1410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>7</v>
       </c>
@@ -1639,7 +1418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>8</v>
       </c>
@@ -1647,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>8</v>
       </c>
@@ -1655,7 +1434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>8</v>
       </c>
@@ -1663,7 +1442,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>8</v>
       </c>
@@ -1671,7 +1450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>8</v>
       </c>
@@ -1679,7 +1458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>8</v>
       </c>
@@ -1687,7 +1466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>8</v>
       </c>
@@ -1695,7 +1474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>8</v>
       </c>
@@ -1703,7 +1482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>8</v>
       </c>
@@ -1711,7 +1490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>8</v>
       </c>
@@ -1719,7 +1498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>8</v>
       </c>
@@ -1727,7 +1506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>8</v>
       </c>
@@ -1735,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>8</v>
       </c>
@@ -1743,7 +1522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>8</v>
       </c>
@@ -1751,7 +1530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>8</v>
       </c>
@@ -1759,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>8</v>
       </c>
@@ -1767,7 +1546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>8</v>
       </c>
@@ -1775,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>8</v>
       </c>
@@ -1783,7 +1562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>8</v>
       </c>
@@ -1791,7 +1570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>8</v>
       </c>
@@ -1799,7 +1578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>8</v>
       </c>
@@ -1807,7 +1586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>8</v>
       </c>
@@ -1815,7 +1594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>8</v>
       </c>
@@ -1823,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>8</v>
       </c>
@@ -1831,7 +1610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>8</v>
       </c>
@@ -1839,7 +1618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>8</v>
       </c>
@@ -1847,7 +1626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>8</v>
       </c>
@@ -1855,7 +1634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>8</v>
       </c>
@@ -1863,7 +1642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>8</v>
       </c>
@@ -1871,7 +1650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>8</v>
       </c>
@@ -1879,7 +1658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>8</v>
       </c>
@@ -1887,7 +1666,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>8</v>
       </c>
@@ -1895,7 +1674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>8</v>
       </c>
@@ -1903,7 +1682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>8</v>
       </c>
@@ -1911,7 +1690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>8</v>
       </c>
@@ -1919,7 +1698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>8</v>
       </c>
@@ -1927,7 +1706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>8</v>
       </c>
@@ -1935,7 +1714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>8</v>
       </c>
@@ -1943,7 +1722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>8</v>
       </c>
@@ -1951,7 +1730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>8</v>
       </c>
@@ -1959,7 +1738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>8</v>
       </c>
@@ -1967,7 +1746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>8</v>
       </c>
@@ -1975,7 +1754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>8</v>
       </c>
@@ -1983,7 +1762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>8</v>
       </c>
@@ -1991,7 +1770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>8</v>
       </c>
@@ -1999,7 +1778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>8</v>
       </c>
@@ -2007,7 +1786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>8</v>
       </c>
@@ -2015,7 +1794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>8</v>
       </c>
@@ -2023,7 +1802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>8</v>
       </c>
@@ -2031,7 +1810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>8</v>
       </c>
@@ -2039,7 +1818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>8</v>
       </c>
@@ -2047,7 +1826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>8</v>
       </c>
@@ -2055,7 +1834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>8</v>
       </c>
@@ -2063,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>9</v>
       </c>
@@ -2071,7 +1850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>9</v>
       </c>
@@ -2079,7 +1858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>9</v>
       </c>
@@ -2087,7 +1866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>9</v>
       </c>
@@ -2095,7 +1874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>9</v>
       </c>
@@ -2103,7 +1882,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>9</v>
       </c>
@@ -2111,7 +1890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>9</v>
       </c>
@@ -2119,7 +1898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>9</v>
       </c>
@@ -2127,7 +1906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>9</v>
       </c>
@@ -2135,7 +1914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>9</v>
       </c>
@@ -2143,7 +1922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>9</v>
       </c>
@@ -2151,7 +1930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>9</v>
       </c>
@@ -2159,7 +1938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>9</v>
       </c>
@@ -2167,7 +1946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>9</v>
       </c>
@@ -2175,7 +1954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>9</v>
       </c>
@@ -2183,7 +1962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>10</v>
       </c>
@@ -2191,7 +1970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>10</v>
       </c>
@@ -2199,7 +1978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>10</v>
       </c>
@@ -2207,7 +1986,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>10</v>
       </c>
@@ -2215,7 +1994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>10</v>
       </c>
@@ -2223,7 +2002,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>10</v>
       </c>
@@ -2231,7 +2010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>10</v>
       </c>
@@ -2239,7 +2018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>10</v>
       </c>
@@ -2247,7 +2026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>10</v>
       </c>
@@ -2255,7 +2034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>10</v>
       </c>
@@ -2263,7 +2042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>10</v>
       </c>
@@ -2271,7 +2050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>10</v>
       </c>
@@ -2279,7 +2058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>10</v>
       </c>
@@ -2287,7 +2066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>10</v>
       </c>
@@ -2295,7 +2074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>11</v>
       </c>
@@ -2303,7 +2082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>11</v>
       </c>
@@ -2311,7 +2090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>11</v>
       </c>
@@ -2319,7 +2098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>11</v>
       </c>
@@ -2327,7 +2106,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>12</v>
       </c>
@@ -2335,7 +2114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>12</v>
       </c>
@@ -2343,7 +2122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>12</v>
       </c>
@@ -2351,7 +2130,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>12</v>
       </c>
@@ -2359,7 +2138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>12</v>
       </c>
@@ -2367,7 +2146,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>12</v>
       </c>
@@ -2375,7 +2154,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>12</v>
       </c>
@@ -2383,7 +2162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>12</v>
       </c>
@@ -2391,7 +2170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>12</v>
       </c>
@@ -2399,7 +2178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>12</v>
       </c>
@@ -2407,7 +2186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>12</v>
       </c>
@@ -2415,7 +2194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>12</v>
       </c>
@@ -2437,39 +2216,38 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="5" max="5" width="7.75" customWidth="1"/>
-    <col min="6" max="6" width="7.25" customWidth="1"/>
+    <col min="5" max="5" width="7.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>202000</v>
@@ -2489,9 +2267,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>96000</v>
@@ -2511,9 +2289,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>67000</v>
@@ -2533,9 +2311,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>76000</v>
@@ -2555,9 +2333,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>123000</v>
@@ -2577,9 +2355,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>154000</v>
@@ -2599,7 +2377,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2621,9 +2399,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B9">
         <v>538000</v>
@@ -2643,9 +2421,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B10">
         <v>150000</v>
@@ -2665,9 +2443,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B11">
         <v>143000</v>
@@ -2687,9 +2465,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <v>47700</v>
@@ -2709,9 +2487,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B13">
         <v>121000</v>
@@ -2731,7 +2509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14">
         <f>SUM(D2:D13)</f>
         <v>202</v>
@@ -2754,15 +2532,53 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:L13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2790,17 +2606,20 @@
       <c r="I2">
         <v>63.6</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="3">
         <v>84</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
         <v>26.04</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <v>27.400000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>57.6</v>
       </c>
@@ -2828,17 +2647,20 @@
       <c r="I3">
         <v>122.80000000000001</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="3">
         <v>132.4</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <v>66</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="3">
         <v>30.200000000000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>25.760000000000005</v>
       </c>
@@ -2866,17 +2688,20 @@
       <c r="I4">
         <v>50.400000000000006</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <v>60</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <v>22.400000000000002</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <v>51.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>47.6</v>
       </c>
@@ -2913,8 +2738,11 @@
       <c r="L5">
         <v>61.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>70</v>
       </c>
@@ -2951,8 +2779,11 @@
       <c r="L6">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>46</v>
       </c>
@@ -2989,8 +2820,11 @@
       <c r="L7">
         <v>53.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>64</v>
       </c>
@@ -3027,8 +2861,11 @@
       <c r="L8">
         <v>36.800000000000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>39.760000000000005</v>
       </c>
@@ -3065,8 +2902,11 @@
       <c r="L9">
         <v>20.560000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>63.6</v>
       </c>
@@ -3103,15 +2943,18 @@
       <c r="L10">
         <v>92.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="M10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>84</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>132.4</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>60</v>
       </c>
       <c r="D11">
@@ -3141,15 +2984,18 @@
       <c r="L11">
         <v>100.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="M11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>26.04</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>66</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>22.400000000000002</v>
       </c>
       <c r="D12">
@@ -3179,15 +3025,18 @@
       <c r="L12">
         <v>35.92</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="M12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>27.400000000000002</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>30.200000000000003</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>51.6</v>
       </c>
       <c r="D13">
@@ -3216,6 +3065,9 @@
       </c>
       <c r="L13">
         <v>0</v>
+      </c>
+      <c r="M13" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3224,490 +3076,708 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D2DD89-6F16-4EE3-9880-A63D62494BDD}">
+  <dimension ref="A2:L13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L13" sqref="A2:L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>57.6</v>
+      </c>
+      <c r="C2">
+        <v>25.760000000000005</v>
+      </c>
+      <c r="D2">
+        <v>47.6</v>
+      </c>
+      <c r="E2">
+        <v>70</v>
+      </c>
+      <c r="F2">
+        <v>46</v>
+      </c>
+      <c r="G2">
+        <v>64</v>
+      </c>
+      <c r="H2">
+        <v>39.760000000000005</v>
+      </c>
+      <c r="I2">
+        <v>63.6</v>
+      </c>
+      <c r="J2" s="3">
+        <v>84</v>
+      </c>
+      <c r="K2" s="3">
+        <v>26.04</v>
+      </c>
+      <c r="L2" s="3">
+        <v>27.400000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>57.6</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>81.600000000000009</v>
+      </c>
+      <c r="D3">
+        <v>91.2</v>
+      </c>
+      <c r="E3">
+        <v>12.440000000000001</v>
+      </c>
+      <c r="F3">
+        <v>82.4</v>
+      </c>
+      <c r="G3">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="H3">
+        <v>50</v>
+      </c>
+      <c r="I3">
+        <v>122.80000000000001</v>
+      </c>
+      <c r="J3" s="3">
+        <v>132.4</v>
+      </c>
+      <c r="K3" s="3">
+        <v>66</v>
+      </c>
+      <c r="L3" s="3">
+        <v>30.200000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>25.760000000000005</v>
+      </c>
+      <c r="B4">
+        <v>81.600000000000009</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>42.800000000000004</v>
+      </c>
+      <c r="E4">
+        <v>94.4</v>
+      </c>
+      <c r="F4">
+        <v>40.800000000000004</v>
+      </c>
+      <c r="G4">
+        <v>83.2</v>
+      </c>
+      <c r="H4">
+        <v>45.2</v>
+      </c>
+      <c r="I4">
+        <v>50.400000000000006</v>
+      </c>
+      <c r="J4" s="3">
+        <v>60</v>
+      </c>
+      <c r="K4" s="3">
+        <v>22.400000000000002</v>
+      </c>
+      <c r="L4" s="3">
+        <v>51.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>47.6</v>
+      </c>
+      <c r="B5">
+        <v>91.2</v>
+      </c>
+      <c r="C5">
+        <v>42.800000000000004</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>94.4</v>
+      </c>
+      <c r="F5">
+        <v>23.680000000000003</v>
+      </c>
+      <c r="G5">
+        <v>77.2</v>
+      </c>
+      <c r="H5">
+        <v>45.2</v>
+      </c>
+      <c r="I5">
+        <v>92.4</v>
+      </c>
+      <c r="J5">
+        <v>45.6</v>
+      </c>
+      <c r="K5">
+        <v>27.680000000000003</v>
+      </c>
+      <c r="L5">
+        <v>61.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>12.440000000000001</v>
+      </c>
+      <c r="C6">
+        <v>94.4</v>
+      </c>
+      <c r="D6">
+        <v>94.4</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>80.800000000000011</v>
+      </c>
+      <c r="G6">
+        <v>25.84</v>
+      </c>
+      <c r="H6">
+        <v>51.2</v>
+      </c>
+      <c r="I6">
+        <v>134.4</v>
+      </c>
+      <c r="J6">
+        <v>142</v>
+      </c>
+      <c r="K6">
+        <v>75.2</v>
+      </c>
+      <c r="L6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>82.4</v>
+      </c>
+      <c r="C7">
+        <v>40.800000000000004</v>
+      </c>
+      <c r="D7">
+        <v>23.680000000000003</v>
+      </c>
+      <c r="E7">
+        <v>80.800000000000011</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>56.400000000000006</v>
+      </c>
+      <c r="H7">
+        <v>32.04</v>
+      </c>
+      <c r="I7">
+        <v>91.2</v>
+      </c>
+      <c r="J7">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="K7">
+        <v>24.040000000000003</v>
+      </c>
+      <c r="L7">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>64</v>
+      </c>
+      <c r="B8">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="C8">
+        <v>83.2</v>
+      </c>
+      <c r="D8">
+        <v>77.2</v>
+      </c>
+      <c r="E8">
+        <v>25.84</v>
+      </c>
+      <c r="F8">
+        <v>56.400000000000006</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>39.360000000000007</v>
+      </c>
+      <c r="I8">
+        <v>129.6</v>
+      </c>
+      <c r="J8">
+        <v>130.4</v>
+      </c>
+      <c r="K8">
+        <v>63.2</v>
+      </c>
+      <c r="L8">
+        <v>36.800000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>39.760000000000005</v>
+      </c>
+      <c r="B9">
+        <v>50</v>
+      </c>
+      <c r="C9">
+        <v>45.2</v>
+      </c>
+      <c r="D9">
+        <v>45.2</v>
+      </c>
+      <c r="E9">
+        <v>51.2</v>
+      </c>
+      <c r="F9">
+        <v>32.04</v>
+      </c>
+      <c r="G9">
+        <v>39.360000000000007</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>95.2</v>
+      </c>
+      <c r="J9">
+        <v>92.800000000000011</v>
+      </c>
+      <c r="K9">
+        <v>25.64</v>
+      </c>
+      <c r="L9">
+        <v>20.560000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>63.6</v>
+      </c>
+      <c r="B10">
+        <v>122.80000000000001</v>
+      </c>
+      <c r="C10">
+        <v>50.400000000000006</v>
+      </c>
+      <c r="D10">
+        <v>92.4</v>
+      </c>
+      <c r="E10">
+        <v>134.4</v>
+      </c>
+      <c r="F10">
+        <v>91.2</v>
+      </c>
+      <c r="G10">
+        <v>129.6</v>
+      </c>
+      <c r="H10">
+        <v>95.2</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>74.8</v>
+      </c>
+      <c r="K10">
+        <v>72</v>
+      </c>
+      <c r="L10">
+        <v>92.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>84</v>
+      </c>
+      <c r="B11" s="3">
+        <v>132.4</v>
+      </c>
+      <c r="C11" s="3">
+        <v>60</v>
+      </c>
+      <c r="D11">
+        <v>45.6</v>
+      </c>
+      <c r="E11">
+        <v>142</v>
+      </c>
+      <c r="F11">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="G11">
+        <v>130.4</v>
+      </c>
+      <c r="H11">
+        <v>92.800000000000011</v>
+      </c>
+      <c r="I11">
+        <v>74.8</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>68</v>
+      </c>
+      <c r="L11">
+        <v>100.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>26.04</v>
+      </c>
+      <c r="B12" s="3">
+        <v>66</v>
+      </c>
+      <c r="C12" s="3">
+        <v>22.400000000000002</v>
+      </c>
+      <c r="D12">
+        <v>27.680000000000003</v>
+      </c>
+      <c r="E12">
+        <v>75.2</v>
+      </c>
+      <c r="F12">
+        <v>24.040000000000003</v>
+      </c>
+      <c r="G12">
+        <v>63.2</v>
+      </c>
+      <c r="H12">
+        <v>25.240000000000002</v>
+      </c>
+      <c r="I12">
+        <v>72</v>
+      </c>
+      <c r="J12">
+        <v>68</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>35.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>27.400000000000002</v>
+      </c>
+      <c r="B13" s="3">
+        <v>30.200000000000003</v>
+      </c>
+      <c r="C13" s="3">
+        <v>51.6</v>
+      </c>
+      <c r="D13">
+        <v>61.6</v>
+      </c>
+      <c r="E13">
+        <v>42</v>
+      </c>
+      <c r="F13">
+        <v>53.2</v>
+      </c>
+      <c r="G13">
+        <v>36.800000000000004</v>
+      </c>
+      <c r="H13">
+        <v>20.560000000000002</v>
+      </c>
+      <c r="I13">
+        <v>92.4</v>
+      </c>
+      <c r="J13">
+        <v>100.4</v>
+      </c>
+      <c r="K13">
+        <v>35.92</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5" style="12" customWidth="1"/>
-    <col min="2" max="2" width="29.25" style="12" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="12" customWidth="1"/>
-    <col min="4" max="4" width="13" style="12" customWidth="1"/>
-    <col min="10" max="10" width="33.5" customWidth="1"/>
+    <col min="1" max="1" width="5.09765625" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="20.8984375" customWidth="1"/>
+    <col min="4" max="4" width="17.09765625" customWidth="1"/>
+    <col min="5" max="5" width="15.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="10"/>
-      <c r="B1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="J1" s="5" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5">
+        <v>100</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="5">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="1"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="23">
-        <f>K31</f>
-        <v>0.2</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="4">
-        <v>16</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="21">
-        <f>K9</f>
-        <v>1664</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" s="4">
-        <v>6</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="25">
-        <f>K40</f>
-        <v>100</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="K5" s="4">
-        <v>6</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="28">
-        <f>K25</f>
-        <v>5</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="J6" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="K6" s="4">
-        <v>1</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" s="4">
-        <v>8</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="5">
-        <f>K3*(K4+K5+K6)*K7</f>
-        <v>1664</v>
-      </c>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="10">
-        <v>1E-4</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J12" s="7"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J13" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="K13" s="6">
-        <v>12</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J14" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="K14" s="6">
-        <f>StedenInformatie!$D$14</f>
-        <v>202</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J15" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="K15" s="6">
-        <f>ROUNDUP(AVERAGE(StedenInformatie!$D$2:$D$13),0)</f>
-        <v>17</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="J16" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="K16" s="6">
-        <v>2</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J18" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="K18" s="7">
-        <f>ROUNDUP(K14/(K13-K16),0)</f>
-        <v>21</v>
-      </c>
-      <c r="L18" s="6"/>
-    </row>
-    <row r="20" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J20" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="K20" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="L20" s="26"/>
-    </row>
-    <row r="21" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-    </row>
-    <row r="22" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J22" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="K22" s="26">
-        <f>K18</f>
-        <v>21</v>
-      </c>
-      <c r="L22" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J23" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="K23" s="26">
-        <v>5</v>
-      </c>
-      <c r="L23" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-    </row>
-    <row r="25" spans="10:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J25" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="K25" s="27">
-        <f>ROUNDUP(K22/K23,0)</f>
-        <v>5</v>
-      </c>
-      <c r="L25" s="26"/>
-    </row>
-    <row r="26" spans="10:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="10:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K27" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="L27" s="9"/>
-    </row>
-    <row r="28" spans="10:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-    </row>
-    <row r="29" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J29" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="K29" s="14">
-        <v>0.19</v>
-      </c>
-      <c r="L29" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-    </row>
-    <row r="31" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J31" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="K31" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="L31" s="8"/>
-    </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J33" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="K33" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="L33" s="17"/>
-      <c r="M33" s="20"/>
-    </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="20"/>
-    </row>
-    <row r="35" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J35" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="K35" s="15">
-        <v>275</v>
-      </c>
-      <c r="L35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="M35" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="N35" s="19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J36" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="K36" s="15">
-        <v>250</v>
-      </c>
-      <c r="L36" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="M36" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="N36" s="19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J37" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="K37" s="15">
-        <v>225</v>
-      </c>
-      <c r="L37" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="M37" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="N37" s="19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J38" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="K38" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="L38" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="M38" s="20"/>
-      <c r="N38" s="19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J39" s="15"/>
-      <c r="K39" s="15"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="19"/>
-    </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J40" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="K40" s="18" cm="1">
-        <f t="array" ref="K40">AVERAGE(K35:K37*K38)</f>
-        <v>100</v>
-      </c>
-      <c r="L40" s="16"/>
-      <c r="M40" s="20"/>
-    </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="M41" s="20"/>
+      <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>